<commit_message>
Add corpus and dictionary for Dictionary-1
</commit_message>
<xml_diff>
--- a/output_dic4.xlsx
+++ b/output_dic4.xlsx
@@ -27856,7 +27856,7 @@
       </c>
       <c r="B1654" s="1" t="inlineStr">
         <is>
-          <t>ལྡེམ་པོ་བཞི། དགོངས་པ་ཅན་བཞི་དང་བརྒྱད་དོ། ལྡེམ་པོར་དགོངས་པ་བཞི་ལ། 1. གཞུག་པ་ལྡེམ་པོར་དགོངས་པ་ནི། འདི་ལྟར་འདུལ་བྱ་འགའ་ཞིག་ཡང་དག་པའི་ལམ་ལ་ཞུགས་པའི་ཆེད་དུ་བརྫུས་ཏེ་བྱུང་བའི་སེམས་ཅན་དང་གཟུགས་ལ་སོགས་པ་ཡོད་པར་གསུངས་པ་ལྟ་བུའོ། 2. མཚན་ཉིད་ལྡེམ་པོར་དགོངས་པ་ནི། ངོ་བོ་ཉིད་གསུམ་ལ་དགོངས་ནས་ཆོས་ཐམས་ཅད་ཡོད་པ་དང་། སྒྱུ་མ་དང་ནམ་མཁའ་དང་འདྲའོ་ཞེས་གསུངས་པ་ལྟ་བུའོ། 3. གཉེན་པོ་ལྡེམ་པོར་དགོངས་པ་ནི། ཉོན་མོངས་པ་རྣམས་ཀྱི་གཉེན་པོར་ཆོས་ཀྱི་སྒོ་མོ་བརྒྱད་ཁྲི་བཞི་སྟོང་བསྟན་པའོ། 4. བསྒྱུར་པ་ལྡེམ་པོར་དགོངས་པ་ནི། དོན་ཟབ་མོའི་ཆེད་དུ་ཡི་གེ་རྣམས་བསྒྱུར་ཏེ་གསུངས་པ་ལྟ་བུའོ། དགོངས་པ་ཅན་བཞི་ལ། 5.ཆོས་སྐུ་མཉམ་པ་ཉིད་ལ་དགོངས་པ་ནི། སངས་རྒྱས་ལ་བརྙས་པའི་གཉེན་པོར་ང་ཉིད་དེའི་ཚེ་དེའི་དུས་ན་སངས་རྒྱས་རྣམ་པར་གཟིགས་སུ་གྱུར་ཏེ་ཞེས་གསུངས་པ་ལྟ་བུའོ། 6. དོན་གཞན་ལ་དགོངས་པ་ནི། ཆོས་བརྙས་པའི་གཉེན་པོར་སངས་རྒྱས་གང་གའི་ཀླུང་གི་བྱེ་མ་རྙེད་ལ་བསྙེན་བཀུར་བྱས་ན་ཆོས་འདི་ཐོས་པར་འགྱུར་ཞེས་པ་ལྟ་བུའོ། 7. དུས་གཞན་ལ་དགོངས་པ་ནི་ལེ་ལོའི་གཉེན་པོར་གང་དག་བརྩོན་འགྲུས་བྱས་ཏེ་བདེ་བ་ཅན་སྨོན་ལམ་འདེབས་པ་དེ་དག་དེར་སྐྱེ་བར་འགྱུར་རོ། ཞེས་པ་ལྟ་བུའོ། 8. གང་ཟག་ལ་བསམ་པ་ལ་དགོངས་པ་ནི། སྦྱིན་པ་ལ་མཆོག་འཛིན་གྱི་གཉེན་པོར། སྦྱིན་པ་ནི་དམན་པ། ཚུལ་ཁྲིམས་ནི་མཆོག་ཅེས་གསུངས་པ་ལྟ་བུའོ།</t>
+          <t>ལྡེམ་པོ་བཞི། དགོངས་པ་ཅན་བཞི་དང་བརྒྱད་དོ། ལྡེམ་པོར་དགོངས་པ་བཞི་ལ། 1. གཞུག་པ་ལྡེམ་པོར་དགོངས་པ་ནི། འདི་ལྟར་འདུལ་བྱ་འགའ་ཞིག་ཡང་དག་པའི་ལམ་ལ་ཞུགས་པའི་ཆེད་དུ་བརྫུས་ཏེ་བྱུང་བའི་སེམས་ཅན་དང་གཟུགས་ལ་སོགས་པ་ཡོད་པར་གསུངས་པ་ལྟ་བུའོ། 2. མཚན་ཉིད་ལྡེམ་པོར་དགོངས་པ་ནི། ངོ་བོ་ཉིད་གསུམ་ལ་དགོངས་ནས་ཆོས་ཐམས་ཅད་ཡོད་པ་དང་། སྒྱུ་མ་དང་ནམ་མཁའ་དང་འདྲའོ་ཞེས་གསུངས་པ་ལྟ་བུའོ། 3. གཉེན་པོ་ལྡེམ་པོར་དགོངས་པ་ནི། ཉོན་མོངས་པ་རྣམས་ཀྱི་གཉེན་པོར་ཆོས་ཀྱི་སྒོ་མོ་བརྒྱད་ཁྲི་བཞི་སྟོང་བསྟན་པའོ། 4. བསྒྱུར་པ་ལྡེམ་པོར་དགོངས་པ་ནི། དོན་ཟབ་མོའི་ཆེད་དུ་ཡི་གེ་རྣམས་བསྒྱུར་ཏེ་གསུངས་པ་ལྟ་བུའོ། དགོངས་པ་ཅན་བཞི་ལ། 5.ཆོས་སྐུ་མཉམ་པ་ཉིད་ལ་དགོངས་པ་ནི། སངས་རྒྱས་ལ་བརྙས་པའི་གཉེན་པོར་ང་ཉིད་དེའི་ཚེ་དེའི་དུས་ན་སངས་རྒྱས་རྣམ་པར་གཟིགས་སུ་གྱུར་ཏེ་ཞེས་གསུངས་པ་ལྟ་བུའོ། 6. དོན་གཞན་ལ་དགོངས་པ་ནི། ཆོས་བརྙས་པའི་གཉེན་པོར་སངས་རྒྱས་གང་གའི་ཀླུང་གི་བྱེ་མ་རྙེད་ལ་བསྙེན་བཀུར་བྱས་ན་ཆོས་འདི་ཐོས་པར་འགྱུར་ཞེས་པ་ལྟ་བུའོ། 7. དུས་གཞན་ལ་དགོངས་པ་ནི་ལེ་ལོའི་གཉེན་པོར་གང་དག་བརྩོན་འགྲུས་བྱས་ཏེ་བདེ་བ་ཅན་སྨོན་ལམ་འདེབས་པ་དེ་དག་དེར་སྐྱེ་བར་འགྱུར་རོ། ཞེས་པ་ལྟ་བུའོ། 8. གང་ཟག་ལ་བསམ་པ་ལ་དགོངས</t>
         </is>
       </c>
       <c r="C1654" s="1" t="inlineStr">
@@ -27890,7 +27890,7 @@
       </c>
       <c r="B1656" s="1" t="inlineStr">
         <is>
-          <t>འདི་ལ་གྲངས་འདྲེན་ཚུལ་མི་འདྲ་བ་འགའ་ཞིག་ཡོད་ཚུལ། འཇམ་དབྱངས་བཞད་པ་དཀོན་མཆོག་འཇིགས་མེད་དབང་པོས་མཛད་པའི་《གསུང་རབ་རྣམས་ལས་བྱུང་བའི་གྲངས་འདྲེན་གྱི་རིམ་པ་ཕྱོགས་གཅིག་ཏུ་བཀོད་པ་》ལས་གསུངས་པ་ལྟར་བྲིས་ན། རྒྱུད་སྡེ་ལས་གསུངས་པའི་སྡེ་བརྒྱད་ནི། 1. ལྷ། 2. ཀླུ། 3. གནོད་སྦྱིན། 4. ལྟོ་འཕྱེ། 5. མཁའ་ལྡིང༌། 6. ལྷ་མིན། 7. བྲུལ་བུམ། 8. མིའམ་ཅི་རྣམས་སོ། ཡང་ལུགས་གཅིག་ལ། 1. དཀར་པོ་ལྷའི་སྡེ། 2. ནག་པོ་བདུད་ཀྱི་སྡེ། 3. དམར་པོ་བཙན་གྱི་སྡེ།	4. སྨུག་པོ་དམུའི་སྡེ། 5. ཁྲ་བོ་གཟའ་ཡི་སྡེ། 6. ཤ་ཟ་སྲིན་པོའི་སྡེ། 7. དཀོར་བདག་རྒྱལ་པོའི་སྡེ། 8. ནད་བདག་མ་མོའི་སྡེ་བཅས་སུ་འདྲེན་ཚུལ་དང་། ཡང་རྙིང་མའི་གཞུང་ལས་གསུངས་པའི་སྡེ་བརྒྱད་གྲངས་འདྲེན་ཚུལ་ཁག་བཞིའི་ནང་ནས་དང་པོ་ཕྱིའི་སྡེ་བརྒྱད་ནི། 1. ལྷ་ཡི་དབང་པོ་བརྒྱ་སྦྱིན། 2. ལྷ་མིན་གྱི་དབང་པོ་ཐགས་བཟང་རིས། 3. ཀླུའི་རྒྱལ་པོ་དགའ་བོ། 4. སྲིན་པོའི་རྒྱལ་པོ་ལང་ཀ་མགྲིན་བཅུ། 5. བདུད་ཀྱི་རྒྱལ་པོ་དམུ་རྗེ་བཙན་པོ། 6. མིའམ་ཅིའི་རྒྱལ་པོ་འཇོན་པ་རྟ་མགོ་ཅན་སོགས། གཉིས་པ། ནང་གི་སྡེ་བརྒྱད་ནི། 1. ཀླུ་སོག་མ་མེད་པ། 2.མ་མོ་ཙ་མུནྚ། 3. གཤིན་རྗེ་དམར་པོ། 4 གཟའ་བདུད་ནག་པོ། 5. བཙན་ཡམ་ཤུད་དམར་པོ། 6. བདུད་མོ་གསེར་མིག་མ། 7. ཡུལ་ལྷ་མ་ཧཱ་དེ་བ། 8. སྨན་མོ་འབྲུག་སྒྲོག གསུམ་པ། གསང་བའི་སྡེ་བརྒྱད་ནི། 1. དབང་ཕྱུག་མ་ཧཱ་དེ་ཝ། 2. ཀླུ་འཆི་བདག་མགོ་དགུ། 3. གཤིན་རྗེ་ཆོས་ཀྱི་རྒྱལ་པོ། 4. མ་མོ་ཨེ་ཀ་ཛཱ་རི། 5. བདུད་པོ་རལ་པ་རྐྱ་གཅིག 6. སྲིན་པོ་ཡཀྵ་ནག་པོ། 7. གནོད་སྦྱིན་སོ་ག 8. གཟའ་ཁྱབ་འཇུག་བཅས་དང་། བཞི་བ། དྲག་པོ་སྔགས་ཀྱི་སྡེ་བརྒྱད་ནི། 1. བཙན་སྤྲུལ་མགོ་ཅན། 2. དམུ་བདུད་ཡ་བ་ཏི། 3. བདུད་ནག་པོ་བཀྲག་མེད། 4. སྲིན་པོ་སྲོག་གཅོད་ནག་པོ། 5. ཀླུ་བདུད་ནག་པོ་སྦྲུལ་ཞགས་ཅན། 6. སྒྲོལ་གྱིང་ཡམ་ཤུད་དམར་པོ། 7. གནོད་སྦྱིན་སྲོག་གཅོད་ནག་པོ། 8. མ་མོ་ནག་པོ་འཇིགས་མ་བཅས་སོ། ད་དུང་དེ་མིན་པའི་འདྲེན་ཚུལ་གཞན་འགའ་ཞིག་ཡོད་ཀྱང་འདིར་མ་བྲིས་སོ།</t>
+          <t>འདི་ལ་གྲངས་འདྲེན་ཚུལ་མི་འདྲ་བ་འགའ་ཞིག་ཡོད་ཚུལ། འཇམ་དབྱངས་བཞད་པ་དཀོན་མཆོག་འཇིགས་མེད་དབང་པོས་མཛད་པའི་《གསུང་རབ་རྣམས་ལས་བྱུང་བའི་གྲངས་འདྲེན་གྱི་རིམ་པ་ཕྱོགས་གཅིག་ཏུ་བཀོད་པ་》ལས་གསུངས་པ་ལྟར་བྲིས་ན། རྒྱུད་སྡེ་ལས་གསུངས་པའི་སྡེ་བརྒྱད་ནི། 1. ལྷ། 2. ཀླུ། 3. གནོད་སྦྱིན། 4. ལྟོ་འཕྱེ། 5. མཁའ་ལྡིང༌། 6. ལྷ་མིན། 7. བྲུལ་བུམ། 8. མིའམ་ཅི་རྣམས་སོ། ཡང་ལུགས་གཅིག་ལ། 1. དཀར་པོ་ལྷའི་སྡེ། 2. ནག་པོ་བདུད་ཀྱི་སྡེ། 3. དམར་པོ་བཙན་གྱི་སྡེ།	4. སྨུག་པོ་དམུའི་སྡེ། 5. ཁྲ་བོ་གཟའ་ཡི་སྡེ། 6. ཤ་ཟ་སྲིན་པོའི་སྡེ། 7. དཀོར་བདག་རྒྱལ་པོའི་སྡེ། 8. ནད་བདག་མ་མོའི་སྡེ་བཅས་སུ་འདྲེན་ཚུལ་དང་། ཡང་རྙིང་མའི་གཞུང་ལས་གསུངས་པའི་སྡེ་བརྒྱད་གྲངས་འདྲེན་ཚུལ་ཁག་བཞིའི་ནང་ནས་དང་པོ་ཕྱིའི་སྡེ་བརྒྱད་ནི། 1. ལྷ་ཡི་དབང་པོ་བརྒྱ་སྦྱིན། 2. ལྷ་མིན་གྱི་དབང་པོ་ཐགས་བཟང་རིས། 3. ཀླུའི་རྒྱལ་པོ་དགའ་བོ། 4. སྲིན་པོའི་རྒྱལ་པོ་ལང་ཀ་མགྲིན་བཅུ། 5. བདུད་ཀྱི་རྒྱལ་པོ་དམུ་རྗེ་བཙན་པོ། 6. མིའམ་ཅིའི་རྒྱལ་པོ་འཇོན་པ་རྟ་མགོ་ཅན་སོགས། གཉིས་པ། ནང་གི་སྡེ་བརྒྱད་ནི། 1. ཀླུ་སོག་མ་མེད་པ། 2.མ་མོ་ཙ་མུནྚ། 3. གཤིན་རྗེ་དམར་པོ། 4 གཟའ་བདུད་ནག་པོ། 5. བཙན་ཡམ་ཤུད་དམར་པོ། 6. བདུད་མོ་གསེར་མིག་མ། 7. ཡུལ་ལྷ་མ་ཧཱ་དེ་བ། 8. སྨན་མོ་འབྲུག་སྒྲོག གསུམ་པ། གསང་བའི་སྡེ་བརྒྱད་ནི། 1. དབང་ཕྱུག་མ་ཧཱ་དེ་ཝ། 2. ཀླུ་འཆི་བདག་མགོ་དགུ། 3. གཤིན་རྗེ་ཆོས་ཀྱི་རྒྱལ་པོ། 4. མ་མོ་ཨེ་ཀ</t>
         </is>
       </c>
       <c r="C1656" s="1" t="inlineStr">
@@ -32662,7 +32662,7 @@
       </c>
       <c r="B1937" s="1" t="inlineStr">
         <is>
-          <t>བྱ་བ་བྱེད་པ་དང་སྡུག་བསྔལ་གྱི་གྲོགས་ཀྱི་དོན་བྱེད་པ། ཐབས་ལ་རྨོངས་པའི་དོན་བྱེད་པ། ཕན་འདོགས་པའི་དོན་བྱེད་པ། འཇིགས་པས་ཉེན་པའི་དོན་བྱེད་པ། མྱ་ངན་གྱིས་གཟིར་བའི་དོན་བྱེད་པ། ཡོ་བྱད་ཀྱིས་འཕོངས་པའི་དོན་བྱེད་པ། གནས་འཆའ་བར་བྱེད་པའི་དོན་བྱེད་པ། བློ་མཐུན་པར་འདོད་པའི་དོན་བྱེད་པ། ཡང་དག་པར་ཞུགས་པའི་དོན་བྱེད་པ། ལོག་པར་ཞུགས་པའི་དོན་བྱེད་པ། རྫུ་འཕྲུལ་གྱི་སྒོ་ནས་གདུལ་བྱའི་དོན་བྱེད་པ་རྣམས་སོ།</t>
+          <t>བྱ་བ་བྱེད་པ་དང་སྡུག་བསྔལ་གྱི་གྲོགས་ཀྱི་དོན་བྱེད་པ། ཐབས་ལ་རྨོངས་པའི་དོན་བྱེད་པ། ཕན་འདོགས་པའི་དོན་བྱེད་པ། འཇིགས་པས་ཉེན་པའི་དོན་བྱེད་པ། མྱ་ངན་གྱིས་གཟིར་བའི་དོན་བྱེད་པ། ཡོ་བྱད་ཀྱིས་འཕོངས་པའི་དོན་བྱེད་པ། གནས་འཆའ་བར་བྱེད་པའི་དོན་བྱེད་པ། བློ</t>
         </is>
       </c>
       <c r="C1937" s="1" t="inlineStr">
@@ -33342,7 +33342,7 @@
       </c>
       <c r="B1977" s="1" t="inlineStr">
         <is>
-          <t>ཉོན་མོངས་སྦྱངས་པའི་ཡོན་ཏན་བཅུ་གཉིས་ཏེ། ཟས་ཀྱི་དབང་དུ་བྱས་པ་གསུམ། གོས་ཀྱི་དབང་དུ་བྱས་པ་གསུམ། གནས་མལ་གྱི་དབང་དུ་བྱས་པ་དྲུག་ཡོད་པའི་ཕྱིར། དང་པོ་གསུམ་ཡོད་དེ། བསོད་སྙོམས་པ་དང༌། སྟན་གཅིག་པ། ཟས་ཕྱིས་མི་ལེན་པ་རྣམས་དེ་ཡིན་པའི་ཕྱིར། དང་པོ་ལ་རྙེད་པས་ཆོག་པའི་བསོད་སྙོམས་པ་དང་། མཐར་གྱིས་སློང་བའི་བསོད་སྙོམས་པ་གཉིས་སུ་ཕྱེ་ནས་སྦྱངས་པའི་ཡོན་ཏན་བཅུ་གསུམ་དུ་བྱས་པ་ཡང་ཡོད་དོ། གོས་ཀྱི་དབང་དུ་བྱས་པ་གསུམ་ཡོད་དེ། ཆོས་གོས་གསུམ་བ་དང༌། ཕྱིང་བ་པ་དང༌། ཕྱག་དར་ཁྲོད་པ་གསུམ་དེ་ཡིན་པའི་ཕྱིར། གནས་མལ་གྱི་དབང་དུ་བྱས་པ་དྲུག་ཡོད་དེ། དགོན་པ་བ་དང༌། ཤིང་དྲུང་པ་དང༌། བླ་གབ་མེད་པ་དང༌། དུར་ཁྲོད་པ་དང༌། ཅོག་བུ་པ་དང༌། གཞི་ཇི་བཞིན་པ་རྣམས་དེ་ཡིན་པའི་ཕྱིར། ཁ་ཅིག་ཕྱི་མ་གཉིས་སྤྱོད་ལམ་གྱི་དབང་དུ་བྱས་པར་མཛད་ནས་གནས་མལ་གྱི་དབང་དུ་བྱས་པ་བཞི་ཡིན་ཞེས་ཟེར། དེ་དག་སོ་སོའི་ངོ་བོ་ཡོད་དེ། རྙེད་པས་ཆོག་པའི་བསོད་སྙོམས་པ་ནི། འདྲེས་པའི་ཁྱིམ་ནས་ཟས་ཇི་ཙམ་རྙེད་པ་ཙམ་ཟ་བར་བྱེད་པ་ཡིན་ལ། མཐར་གྱིས་སློང་བའི་བསོད་སྙོམས་པ་ནི། ཁྱིམ་རྣམས་སུ་རིམ་གྱིས་བརྒྱུས་ཏེ་བསོད་སྙོམས་ཇི་ཙམ་རྙེད་པ་ཟ་བར་བྱེད་ཀྱི། བདག་གིས་འདི་ནས་བཟའ་བ་དང་བཅའ་བ་བཟང་པོ་འཐོབ་བོ་སྙམ་ནས། མགོ་འཕང་བསྟོད་དེ་མི་འགྲོ་བའོ། སྟན་གཅིག་པ་ནི། སྟན་གཅིག་པོ་དེ་ལ་འདུག་ནས་ཇི་ཙམ་ཟ་བ་དེ་ཙམ་དུ་ཟ་བར་བྱེད་ཀྱི། དེ་ལས་ལངས་ནས་མི་ཟ་བའོ། ཟས་ཕྱིས་མི་ལེན་པ་ནི། ཟས་ཀྱི་ཕྱིར་འདུག་ནས་ཇི་ཙམ་གྱིས་བདག་འཚོ་བའི་ཟས་ཐམས་ཅད་མ་བླངས་ཀྱི་བར་དུ་མི་ཟ་ཞིང་འདིས་འཚོའོ་སྙམ་པ་དང་ཐམས་ཅད་ཅིག་ཆར་བླངས་ན་ཟ་བའོ། ཆོས་གོས་གསུམ་པ་ནི། སྣམ་སྦྱར། བླ་གོས། མཐང་གོས་གསུམ་གྱིས་འཚོ་བར་བྱེད་ཅིང་དེ་ལས་ལྷག་པའི་གོས་མི་འཆང་བ་དང་། ཕྱིང་བ་པ་ནི། ཆོས་གོས་གསུམ་མམ་གོས་ལྷག་ཅི་འཆང་བ་ཐམས་ཅད་བལ་ལས་བྱས་པ་ཤ་སྟག་འཆང་གི་དེ་ལས་གཞན་མི་འཆང་བ་དང་། ཕྱག་དར་ཁྲོད་པ་ནི། ལམ་པོ་ཆེ་ལ་སོགས་པར་བོར་བའི་གོས་གཤང་གཅི་སོགས་ཀྱིས་རེག་པ་མི་གཙང་བ་རྣམས་བོར་ཏེ་རུང་བ་བླངས་ཏེ་བཀྲུས་དྲུབ་ཁ་དོག་བཟང་བོར་བསྒྱུར་ནས་འཆང་བར་བྱེད་པ་དང་། དགོན་པ་བ་ནི། གྲོང་དང་གྲོང་རྡལ་ལ་སོགས་པས་དབེན་པའི་དགོན་པ་དང་ནགས་འདབ་ལ་སོགས་པར་གནས་པ་དང་། ཤིང་དྲུང་པ་ནི། ཤིང་ལྗོན་པའི་དྲུང་དུ་གནས་འཆའ་ཞིང་བརྟེན་པར་བྱེད་པ་དང༌། བླ་གབ་མེད་པ་ནི། སྟེང་གི་ཐོག་མ་བཀབ་ཅིང་མ་གཡོགས་པའི་ཕྱོགས་སུ་གནས་འཆའ་བར་བྱེད་པ་དང༌། དུར་ཁྲོད་པ་ནི། གང་དུ་སྐྱེ་བོ་ཤིའོ་ཅོག་འདོར་བའི་དུར་ཁྲོད་དུ་གནས་འཆའ་བར་བྱེད་པ་དང་། ཅོག་བུ་པ་ནི། ཁྲིའམ། ཁྲིའུའམ། རྩྭའི་སྟེང་དུ་ཅོག་བུར་འདུག་སྟེ་ཁྲི་ལ་སོགས་པ་ལ་རྒྱབ་བམ་གློས་མི་བརྟེན་པ་དང་། གཞི་ཇི་བཞིན་པ་ནི། རྩྭ་དང་ལོ་མ་ལ་སོགས་པ་བཏིང་བ་མལ་ལ་འཆའ་ཞིང་ལན་ཅིག་ཇི་ལྟར་བཏིང་བ་ལ་མལ་འཆའ་བར་བྱེད་ཀྱི། ཡང་དང་ཡང་དུ་མི་བརྗེ་ཞིང་མི་འཆོས་པའོ། དེ་དག་ནི་ཉན་ཐོས་ཀྱི་ས་ལས་ཇི་ལྟར་འབྱུང་བ་བཞིན་ཡིན་ནོ། ཡང་ཞིང་པ་བ་མ་གཏོགས་པ་རྣམས་ལ་ཆུང་ངུ་། འབྲིང་། ཆེན་པོ་གསུམ་གསུམ་ཡོད་དེ། བསོད་སྙོམས་པ་ལ་གསུམ་ལས། པར་གནས་པ་དང་། ། ཆེན་པོ་ནི། སྟེང་གི་ངོས་ཐམས་ཅད་མ་གཡོགས་པར་གནས་པའོ། དུར་ཁྲོད་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། སྔོན་དུར་ཁྲོད་ཡིན་ལ་ད་ལྟ་དུར་ཁྲོད་མ་ཡིན་པར་གནས་པ་དང༌། ། འབྲིང་ནི། རོ་ཅུང་ཟད་སྐྱེལ་བའི་སར་གནས་པ་དང་། ཆེན་པོ་ནི། སྐྱེ་བོ་ཤིའོ་ཅོག་སྐྱེལ་པའི་སར་གནས་པའོ། ཅོག་བུ་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ངོས་གཉིས་བསྙེས་ནས་གནས་པ་དང༌། འབྲིང་ནི། ངོས་གཅིག་བསྙེས་ནས་གནས་པ་དང༌། ཆེན་པོ་ནི། ངོས་ཐམས་ཅད་མ་བསྙེས་པར་གནས་པའོ། གཞི་ཇི་བཞིན་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ། ལན་གསུམ་དུ་མལ་འཆའི། གཞན་མི་བྱེད་པ་དང༌། འབྲིང་ནི། ལན་གཉིས་སུ་མལ་འཆའི། གཞན་མི་བྱེད་པ་དང་། ཆེན་པོ་ནི། ལན་གཅིག་སྟན་བཏིང་བ་ལ་མལ་འཆའི། ཡང་དང་ཡང་དུ་མི་བརྗེ་མི་འཆོས་པའོ། དེ་དག་ལ་ཅིའི་ཕྱིར་སྦྱངས་པའི་ཡོན་ཏན་ཞེས་བྱ་ཞེ་ན། དཔེར་ན་བལ་མ་སྨེལ་བ་དེའི་ཚེ་སྐུད་པ་མི་རུང་ལ་སྨེལ་ནས་རུང་བ་བཞིན་དུ་བསོད་སྙོམས་དང་ཆོས་གོས་དང་གནས་མལ་ལ་ཆགས་པའི་ཚེ་སེམས་ལས་སུ་མི་རུང་ལ། ཡོན་ཏན་འ་དི་དག་གིས་ཚངས་སྤྱོད་གནས་པར་བྱ་བའི་ཕྱིར་སེམས་ལས་རུང་དུ་སྦྱོར་བར་བྱེད་པའི་ཕྱིར་དེ་སྐད་ཅེས་བྱའོ། ཆེན་པོ་ནི། ཆོས་གོས་གསུམ་ཙམ་འཆང་གི་དེ་ལས་ལྷག་པ་མི་འཆང་པའོ།། ཕྱག་དར་ཁྲོད་པ་ལ་ཡང་གསུ་མ་ལས། ཆུང་ངུ་ནི། བྱི་བས་ཟོས་པ་ཚིག་པ་དུམ་བུར་བཅད་པ་གཞན་གྱིས་རང་གི་ཆེད་དུ་བྱས་པ་ལེན་པ་དང་། འབྲིང་ནི། རང་གི་ཆེད་དུ་བྱས་པ་མི་ལེན་པར་མ་ངེས་པར་བོར་བ་ལེན་པ་དང༌། ཆེན་པོ་ནི། དེ་དག་ལེན་པར་དུར་ཁྲོད་དང་ཕྱག་དར་ཁྲོད་དང་ལམ་པོ་ཆེར་ལྷུང་བ་ལེན་པ། དགོན་པ་བ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། གྲོང་ལས་གཞུ་འདོམ་ལྔ་བརྒྱས་བཅད་པའི་སར་གནས་པ་དང༌། འབྲིང་ནི་གྲོང་ལས་གཞུ་འདོམ་སྟོང་ཕྲག་གཉིས་ཀྱིས་བཅད་པའི་སར་གནས་པ་དང༌། ཆེན་པོ་ནི། གྲོང་ལས་གཞུ་འདོམ་སྟོང་ཕྲག་བརྒྱད་ཀྱིས་བཅད་པའི་སར་གནས་པའོ། ཤིང་དྲུང་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ཤིང་དྲུང་ངོས་བཞི་བོ་ཐམས་ཅད་སྐྱོར་བར་གནས་པ་དང༌། འབྲིང་ནི། དེར་ངོས་ཅུང་ཟད་སྐྱོར་བར་གནས་པ་དང༌། ཆེན་པོ་ནི། དེར་ངོས་ཐམས་ཅད་མ་སྐྱོར་བར་གནས་པའོ། བླ་གབ་མེད་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། སྟེང་གི་ངོས་གསུམ་གཡོགས་ལ་གཅིག་མ་གཡོགས་པར་གནས་པ་དང༌། འབྲིང་ནི། སྟེང་གི་ངོས་གཅིག་གཡོགས་ལ་གསུམ་མ་གཡོགས་པར་གནས་པ་དང་། ཆེན་པོ་ནི། སྟེང་གི་ངོས་ཐམས་ཅད་མ་གཡོགས་པར་གནས་པའོ། ། དུར་ཁྲོད་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ། སྔོན་དུར་ཁྲོད་ཡིན་ལ་ད་ལྟ་དུར་ཁྲོད་མ་ཡིན་པར་གནས་པ་དང༌། འབྲིང་ནི། རོ་ཅུང་ཟད་སྐྱེལ་བའི་སར་གནས་པ་དང༌། ཆེན་པོ་ནི། སྐྱེ་བོ་ཤིའོ་ཅོག་སྐྱེལ་པའི་སར་གནས་པའོ། ཅོག་བུ་བ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ངོས་གཉིས་བསྙེས་ནས་གནས་པ་དང་། འབྲིང་ནི། ངོས་གཅིག་བསྙེས་ནས་གནས་པ་དང༌། ཆེན་པོ་ནི། ངོས་ཐམས་ཅད་མ་བསྙེས་པར་གནས་པའོ། གཞི་ཇི་བཞིན་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ལན་གསུམ་དུ་མལ་འཆའི། གཞན་མི་བྱེད་པ་དང་། འབྲིང་ནི། ལན་གཉིས་སུ་མལ་འཆའི། གཞན་མི་བྱེད་པ་དང་། ཆེན་པོ་ནི། ལན་གཅིག་སྟན་བཏིང་བ་ལ་མལ་འཆའི་། ཡང་དང་ཡང་དུ་མི་བརྗེ་མི་འཆོས་པའོ། དེ་དག་ལ་ཅིའི་ཕྱིར་སྦྱངས་པའི་ཡོན་ཏན་ཞེས་བྱ་ཞེ་ན། ། དཔེར་ན་བལ་མ་སྨེལ་བ་དེའི་ཚེ་སྐུད་པ་མི་རུང་ལ་སྨེལ་ནས་རུང་བ་བཞིན་དུ་བསོད་སྙོམས་དང་ཆོས་གོས་དང་གནས་མལ་ལ་ཆགས་པའི་ཚེ་སེམས་ལས་སུ་མི་རུང་ལ། ཡོན་ཏན་འ་དི་དག་གིས་ཚངས་སྤྱོད་གནས་པར་བྱ་བའི་ཕྱིར་སེམས་ལས་རུང་དུ་སྦྱོར་བར་བྱེད་པའི་ཕྱིར་དེ་སྐད་ཅེས་བྱའོ།</t>
+          <t>ཉོན་མོངས་སྦྱངས་པའི་ཡོན་ཏན་བཅུ་གཉིས་ཏེ། ཟས་ཀྱི་དབང་དུ་བྱས་པ་གསུམ། གོས་ཀྱི་དབང་དུ་བྱས་པ་གསུམ། གནས་མལ་གྱི་དབང་དུ་བྱས་པ་དྲུག་ཡོད་པའི་ཕྱིར། དང་པོ་གསུམ་ཡོད་དེ། བསོད་སྙོམས་པ་དང༌། སྟན་གཅིག་པ། ཟས་ཕྱིས་མི་ལེན་པ་རྣམས་དེ་ཡིན་པའི་ཕྱིར། དང་པོ་ལ་རྙེད་པས་ཆོག་པའི་བསོད་སྙོམས་པ་དང་། མཐར་གྱིས་སློང་བའི་བསོད་སྙོམས་པ་གཉིས་སུ་ཕྱེ་ནས་སྦྱངས་པའི་ཡོན་ཏན་བཅུ་གསུམ་དུ་བྱས་པ་ཡང་ཡོད་དོ། གོས་ཀྱི་དབང་དུ་བྱས་པ་གསུམ་ཡོད་དེ། ཆོས་གོས་གསུམ་བ་དང༌། ཕྱིང་བ་པ་དང༌། ཕྱག་དར་ཁྲོད་པ་གསུམ་དེ་ཡིན་པའི་ཕྱིར། གནས་མལ་གྱི་དབང་དུ་བྱས་པ་དྲུག་ཡོད་དེ། དགོན་པ་བ་དང༌། ཤིང་དྲུང་པ་དང༌། བླ་གབ་མེད་པ་དང༌། དུར་ཁྲོད་པ་དང༌། ཅོག་བུ་པ་དང༌། གཞི་ཇི་བཞིན་པ་རྣམས་དེ་ཡིན་པའི་ཕྱིར། ཁ་ཅིག་ཕྱི་མ་གཉིས་སྤྱོད་ལམ་གྱི་དབང་དུ་བྱས་པར་མཛད་ནས་གནས་མལ་གྱི་དབང་དུ་བྱས་པ་བཞི་ཡིན་ཞེས་ཟེར། དེ་དག་སོ་སོའི་ངོ་བོ་ཡོད་དེ། རྙེད་པས་ཆོག་པའི་བསོད་སྙོམས་པ་ནི། འདྲེས་པའི་ཁྱིམ་ནས་ཟས་ཇི་ཙམ་རྙེད་པ་ཙམ་ཟ་བར་བྱེད་པ་ཡིན་ལ། མཐར་གྱིས་སློང་བའི་བསོད་སྙོམས་པ་ནི། ཁྱིམ་རྣམས་སུ་རིམ་གྱིས་བརྒྱུས་ཏེ་བསོད་སྙོམས་ཇི་ཙམ་རྙེད་པ་ཟ་བར་བྱེད་ཀྱི། བདག་གིས་འདི་ནས་བཟའ་བ་དང་བཅའ་བ་བཟང་པོ་འཐོབ་བོ་སྙམ་ནས། མགོ་འཕང་བསྟོད་དེ་མི་འགྲོ་བའོ། སྟན་གཅིག་པ་ནི། སྟན་གཅིག་པོ་དེ་ལ་འདུག་ནས་ཇི་ཙམ་ཟ་བ་དེ་ཙམ་དུ་ཟ་བར་བྱེད་ཀྱི། དེ་ལས་ལངས་ནས་མི་ཟ་བའོ། ཟས་ཕྱིས་མི་ལེན་པ་ནི། ཟས་ཀྱི་ཕྱིར་འདུག་ནས་ཇི་ཙམ་གྱིས་བདག་འཚོ་བའི་ཟས་ཐམས་ཅད་མ་བླངས་ཀྱི་བར་དུ་མི་ཟ་ཞིང་འདིས་འཚོའོ་སྙམ་པ་དང་ཐམས་ཅད་ཅིག་ཆར་བླངས་ན་ཟ་བའོ། ཆོས་གོས་གསུམ་པ་ནི། སྣམ་སྦྱར། བླ་གོས། མཐང་གོས་གསུམ་གྱིས་འཚོ་བར་བྱེད་ཅིང་དེ་ལས་ལྷག་པའི་གོས་མི་འཆང་བ་དང་། ཕྱིང་བ་པ་ནི། ཆོས་གོས་གསུམ་མམ་གོས་ལྷག་ཅི་འཆང་བ་ཐམས་ཅད་བལ་ལས་བྱས་པ་ཤ་སྟག་འཆང་གི་དེ་ལས་གཞན་མི་འཆང་བ་དང་། ཕྱག་དར་ཁྲོད་པ་ནི། ལམ་པོ་ཆེ་ལ་སོགས་པར་བོར་བའི་གོས་གཤང་གཅི་སོགས་ཀྱིས་རེག་པ་མི་གཙང་བ་རྣམས་བོར་ཏེ་རུང་བ་བླངས་ཏེ་བཀྲུས་དྲུབ་ཁ་དོག་བཟང་བོར་བསྒྱུར་ནས་འཆང་བར་བྱེད་པ་དང་། དགོན་པ་བ་ནི། གྲོང་དང་གྲོང་རྡལ་ལ་སོགས་པས་དབེན་པའི་དགོན་པ་དང་ནགས་འདབ་ལ་སོགས་པར་གནས་པ་དང་། ཤིང་དྲུང་པ་ནི། ཤིང་ལྗོན་པའི་དྲུང་དུ་གནས་འཆའ་ཞིང་བརྟེན་པར་བྱེད་པ་དང༌། བླ་གབ་མེད་པ་ནི། སྟེང་གི་ཐོག་མ་བཀབ་ཅིང་མ་གཡོགས་པའི་ཕྱོགས་སུ་གནས་འཆའ་བར་བྱེད་པ་དང༌། དུར་ཁྲོད་པ་ནི། གང་དུ་སྐྱེ་བོ་ཤིའོ་ཅོག་འདོར་བའི་དུར་ཁྲོད་དུ་གནས་འཆའ་བར་བྱེད་པ་དང་། ཅོག་བུ་པ་ནི། ཁྲིའམ། ཁྲིའུའམ། རྩྭའི་སྟེང་དུ་ཅོག་བུར་འདུག་སྟེ་ཁྲི་ལ་སོགས་པ་ལ་རྒྱབ་བམ་གློས་མི་བརྟེན་པ་དང་། གཞི་ཇི་བཞིན་པ་ནི། རྩྭ་དང་ལོ་མ་ལ་སོགས་པ་བཏིང་བ་མལ་ལ་འཆའ་ཞིང་ལན་ཅིག་ཇི་ལྟར་བཏིང་བ་ལ་མལ་འཆའ་བར་བྱེད་ཀྱི། ཡང་དང་ཡང་དུ་མི་བརྗེ་ཞིང་མི་འཆོས་པའོ། དེ་དག་ནི་ཉན་ཐོས་ཀྱི་ས་ལས་ཇི་ལྟར་འབྱུང་བ་བཞིན་ཡིན་ནོ། ཡང་ཞིང་པ་བ་མ་གཏོགས་པ་རྣམས་ལ་ཆུང་ངུ་། འབྲིང་། ཆེན་པོ་གསུམ་གསུམ་ཡོད་དེ། བསོད་སྙོམས་པ་ལ་གསུམ་ལས། པར་གནས་པ་དང་། ། ཆེན་པོ་ནི། སྟེང་གི་ངོས་ཐམས་ཅད་མ་གཡོགས་པར་གནས་པའོ། དུར་ཁྲོད་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། སྔོན་དུར་ཁྲོད་ཡིན་ལ་ད་ལྟ་དུར་ཁྲོད་མ་ཡིན་པར་གནས་པ་དང༌། ། འབྲིང་ནི། རོ་ཅུང་ཟད་སྐྱེལ་བའི་སར་གནས་པ་དང་། ཆེན་པོ་ནི། སྐྱེ་བོ་ཤིའོ་ཅོག་སྐྱེལ་པའི་སར་གནས་པའོ། ཅོག་བུ་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ངོས་གཉིས་བསྙེས་ནས་གནས་པ་དང༌། འབྲིང་ནི། ངོས་གཅིག་བསྙེས་ནས་གནས་པ་དང༌། ཆེན་པོ་ནི། ངོས་ཐམས་ཅད་མ་བསྙེས་པར་གནས་པའོ། གཞི་ཇི་བཞིན་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ། ལན་གསུམ་དུ་མལ་འཆའི། གཞན་མི་བྱེད་པ་དང༌། འབྲིང་ནི། ལན་གཉིས་སུ་མལ་འཆའི། གཞན་མི་བྱེད་པ་དང་། ཆེན་པོ་ནི། ལན་གཅིག་སྟན་བཏིང་བ་ལ་མལ་འཆའི། ཡང་དང་ཡང་དུ་མི་བརྗེ་མི་འཆོས་པའོ། དེ་དག་ལ་ཅིའི་ཕྱིར་སྦྱངས་པའི་ཡོན་ཏན་ཞེས་བྱ་ཞེ་ན། དཔེར་ན་བལ་མ་སྨེལ་བ་དེའི་ཚེ་སྐུད་པ་མི་རུང་ལ་སྨེལ་ནས་རུང་བ་བཞིན་དུ་བསོད་སྙོམས་དང་ཆོས་གོས་དང་གནས་མལ་ལ་ཆགས་པའི་ཚེ་སེམས་ལས་སུ་མི་རུང་ལ། ཡོན་ཏན་འ་དི་དག་གིས་ཚངས་སྤྱོད་གནས་པར་བྱ་བའི་ཕྱིར་སེམས་ལས་རུང་དུ་སྦྱོར་བར་བྱེད་པའི་ཕྱིར་དེ་སྐད་ཅེས་བྱའོ། ཆེན་པོ་ནི། ཆོས་གོས་གསུམ་ཙམ་འཆང་གི་དེ་ལས་ལྷག་པ་མི་འཆང་པའོ།། ཕྱག་དར་ཁྲོད་པ་ལ་ཡང་གསུ་མ་ལས། ཆུང་ངུ་ནི། བྱི་བས་ཟོས་པ་ཚིག་པ་དུམ་བུར་བཅད་པ་གཞན་གྱིས་རང་གི་ཆེད་དུ་བྱས་པ་ལེན་པ་དང་། འབྲིང་ནི། རང་གི་ཆེད་དུ་བྱས་པ་མི་ལེན་པར་མ་ངེས་པར་བོར་བ་ལེན་པ་དང༌། ཆེན་པོ་ནི། དེ་དག་ལེན་པར་དུར་ཁྲོད་དང་ཕྱག་དར་ཁྲོད་དང་ལམ་པོ་ཆེར་ལྷུང་བ་ལེན་པ། དགོན་པ་བ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། གྲོང་ལས་གཞུ་འདོམ་ལྔ་བརྒྱས་བཅད་པའི་སར་གནས་པ་དང༌། འབྲིང་ནི་གྲོང་ལས་གཞུ་འདོམ་སྟོང་ཕྲག་གཉིས་ཀྱིས་བཅད་པའི་སར་གནས་པ་དང༌། ཆེན་པོ་ནི། གྲོང་ལས་གཞུ་འདོམ་སྟོང་ཕྲག་བརྒྱད་ཀྱིས་བཅད་པའི་སར་གནས་པའོ། ཤིང་དྲུང་པ་ལ་ཡང་གསུམ་ལས། ཆུང་ངུ་ནི། ཤིང་དྲུང་ངོས་བཞི་བོ་ཐམས་ཅད་སྐྱོར་བར་གནས་པ་དང༌། འབྲིང་ནི། དེར་ངོས་ཅུང་ཟད་སྐྱོར་</t>
         </is>
       </c>
       <c r="C1977" s="1" t="inlineStr">
@@ -33920,7 +33920,7 @@
       </c>
       <c r="B2011" s="1" t="inlineStr">
         <is>
-          <t>1. རྗེ་དུས་གསུམ་མཁྱེན་པ། (རབ་བྱུང་གཉིས་པའི་ལྕགས་སྟག་སྤྱི་ལོ་1110—རབ་བྱུང་གསུམ་པའི་ཆུ་གླང་སྤྱི་ལོ་1193བར)འཁྲུངས་ཡུལ་མདོ་ཁམས་ཀྲེ་ཤོད། དགུང་ལོ་བརྒྱད་ཅུ་གྱ་བཞི་བཞུགས། 2. ཀརྨ་པཀྴི་ཆོས་ཀྱི་བླ་མ། (རབ་བྱུང་གསུམ་པའི་ཤིང་བྱི་སྤྱི་ལོ་1204—རབ་བྱུང་ལྔ་པའི་ཆུ་ལུག་སྤྱི་ལོ་1283བར)དགུང་ལོ་དོན་དགུ་བཞུགས། 3. ཀརྨ་པ་རང་བྱུང་རྡོ་རྗེ། (རབ་བྱུང་ལྔ་པའི་ཤིང་སྤྲེལ་སྤྱི་ལོ་1284—རབ་བྱུང་དྲུག་པའི་ས་ཡོས་སྤྱི་ལོ་1339བར)དགུང་ལོ་ང་དྲུག་བཞུགས། 4. ཀརྨ་པ་རོལ་པའི་རྡོ་རྗེ། (རབ་བྱུང་དྲུག་པའི་ལྕགས་འབྲུག་སྤྱི་ལོ་1340—རབ་བྱུང་དྲུག་པའི་ཆུ་ཕག་སྤྱི་ལོ་1383བར）དགུང་ལོ་ཞེ་བཞི་བཞུགས།5. ཀརྨ་པ་དེ་བཞིན་གཤེགས་པ།（རབ་བྱུང་དྲུག་པའི་ཤིང་བྱི་སྤྱི་ལོ་ 1384—རབ་བྱུང་བདུན་པའི་ཤིང་ལུག་སྤྱི་ལོ་1415 བར)དགུང་ལོ་སོ་གཉིས་བཞུགས།6. ཀརྨ་པ་མཐོང་བ་དོན་ལྡན(རབ་བྱུང་བདུན་པའི་མེ་སྤྲེལ་སྤྱི་ལོ་1416—རབ་བྱུང་བརྒྱད་པའི་ཆུ་བྱ་སྤྱི་ལོ་1453བར)དགུང་ལོ་སོ་བརྒྱད་བཞུགས། 7. ཀརྨ་པ་ཆོས་གྲགས་རྒྱ་མཚོ། (རབ་བྱུང་བརྒྱད་པའི་ཤིང་ཁྱི་སྤྱི་ལོ་ 1454—རབ་བྱུང་བརྒྱད་པའི་མེ་སྟག་སྤྱི་ལོ་1506 བར）དགུང་ལོ་ང་གསུམ་བཞུགས།8. ཀརྨ་པ་མི་བསྐྱོད་རྡོ་རྗེ། (རབ་བྱུང་དགུ་པའི་མེ་ཡོས་སྤྱི་ལོ་1507—རབ་བྱུང་དགུ་པའི་ཤིང་སྟག་སྤྱི་ལོ་1554བར）དགུང་ལོ་ཞེ་བརྒྱད་བཞུགས།9. ཀརྨ་པ་དབང་ཕྱུག་རྡོ་རྗེ། (རབ་བྱུང་དགུ་པའི་མེ་འབྲུག་སྤྱི་ལོ་1556—རབ་བྱུང་བཅུ་པའི་ཆུ་ཡོས་སྤྱི་ལོ་1603བར）དགུང་ལོ་ཞེ་བརྒྱད་བཞུགས།10. ཀརྨ་པ་ཆོས་དབྱིངས་རྡོ་རྗེ། (རབ་བྱུང་བཅུ་པའི་ཤིང་འབྲུག་སྤྱི་ལོ་1604—རབ་བྱུང་བཅུ་གཅིག་པའི་ཤིང་སྟག་སྤྱི་ལོ་1674བར) དགུང་ལོ་དོན་གཅིག་བཞུགས།11. ཀརྨ་པ་ཡེ་ཤེས་རྡོ་རྗེ། (རབ་བྱུང་བཅུ་གཅིག་པའི་མེ་སྦྲུལ་སྤྱི་ལོ་1677—རབ་བྱུང་བཅུ་གཉིས་པའི་ལྕགས་སྦྲུལ་སྤྱི་ལོ་1701 བར）དགུང་ལོ་ཉེར་ལྔ་བཞུགས།12. ཀརྨ་པ་བྱང་ཆུབ་རྡོ་རྗེ། (རབ་བྱུང་བཅུ་གཉིས་པའི་ཆུ་རྟ་སྤྱི་ལོ་1702—རབ་བྱུང་བཅུ་གཉིས་པའི་ཆུ་བྱི་སྤྱི་ལོ་1732བར) དགུང་ལོ་སོ་གཅིག་བཞུགས།13. ཀརྨ་བ་བདུད་འདུལ་རྡོ་རྗེ། (རབ་བྱུང་བཅུ་གཉིས་པའི་ཆུ་གླང་སྤྱི་ལོ་1733-) དགུང་ལོ?། 14. ཀརྨ་པ་ཐེག་མཆོག་རྡོ་རྗེ།（རབ་བྱུང་བཅུ་གསུམ་པའི་མེ་སྦྲུལ་སྤྱི་ལོ་1797——?） དགུང་ལོ ? བཅས།</t>
+          <t>1. རྗེ་དུས་གསུམ་མཁྱེན་པ། (རབ་བྱུང་གཉིས་པའི་ལྕགས་སྟག་སྤྱི་ལོ་1110—རབ་བྱུང་གསུམ་པའི་ཆུ་གླང་སྤྱི་ལོ་1193བར)འཁྲུངས་ཡུལ་མདོ་ཁམས་ཀྲེ་ཤོད། དགུང་ལོ་བརྒྱད་ཅུ་གྱ་བཞི་བཞུགས། 2. ཀརྨ་པཀྴི་ཆོས་ཀྱི་བླ་མ། (རབ་བྱུང་གསུམ་པའི་ཤིང་བྱི་སྤྱི་ལོ་1204—རབ་བྱུང་ལྔ་པའི་ཆུ་ལུག་སྤྱི་ལོ་1283བར)དགུང་ལོ་དོན་དགུ་བཞུགས། 3. ཀརྨ་པ་རང་བྱུང་རྡོ་རྗེ། (རབ་བྱུང་ལྔ་པའི་ཤིང་སྤྲེལ་སྤྱི་ལོ་1284—རབ་བྱུང་དྲུག་པའི་ས་ཡོས་སྤྱི་ལོ་1339བར)དགུང་ལོ་ང་དྲུག་བཞུགས། 4. ཀརྨ་པ་རོལ་པའི་རྡོ་རྗེ། (རབ་བྱུང་དྲུག་པའི་ལྕགས་འབྲུག་སྤྱི་ལོ་1340—རབ་བྱུང་དྲུག་པའི་ཆུ་ཕག་སྤྱི་ལོ་1383བར）དགུང་ལོ་ཞེ་བཞི་བཞུགས།5. ཀརྨ་པ་དེ་བཞིན་གཤེགས་པ།（རབ་བྱུང་དྲུག་པའི་ཤིང་བྱི་སྤྱི་ལོ་ 1384—རབ་བྱུང་བདུན་པའི་ཤིང་ལུག་སྤྱི་ལོ་1415 བར)དགུང་ལོ་སོ་གཉིས་བཞུགས།6. ཀརྨ་པ་མཐོང་བ་དོན་ལྡན(རབ་བྱུང་བདུན་པའི་མེ་སྤྲེལ་སྤྱི་ལོ་1416—རབ་བྱུང་བརྒྱད་པའི་ཆུ་བྱ་སྤྱི་ལོ་1453བར)དགུང་ལོ་སོ་བརྒྱད་བཞུགས། 7. ཀརྨ་པ་ཆོས་གྲགས་རྒྱ་མཚོ། (རབ་བྱུང་བརྒྱད་པའི་ཤིང་ཁྱི་སྤྱི་ལོ་ 1454—རབ་བྱུང་བརྒྱད་པའི་མེ་སྟག་སྤྱི་ལོ་1506 བར）དགུང་ལོ་ང་གསུམ་བཞུགས།8. ཀརྨ་པ་མི་བསྐྱོད་རྡོ་རྗེ། (རབ་བྱུང་དགུ་པའི་མེ་ཡོས་སྤྱི་ལོ་1507—རབ་བྱུང་དགུ་པའི་ཤིང་སྟག་སྤྱི་ལོ་1554བར）དགུང་ལོ་ཞེ་བརྒྱད་བཞུགས།9. ཀརྨ་པ་དབང་ཕྱུག་རྡོ་རྗ</t>
         </is>
       </c>
       <c r="C2011" s="1" t="inlineStr">
@@ -33988,7 +33988,7 @@
       </c>
       <c r="B2015" s="1" t="inlineStr">
         <is>
-          <t>གུར་ལས་དམ་ཚིག་བཅུ་བཞི་གསུངས་ཏེ། 1. དཀོན་མཆོག་མི་སྤང་། 2. དམ་ཚིག་རྟག་ཏུ་སྤྱད། 3. རྡོར་དྲིལ། 4. གཙུག་ཏོར་འཆང་དང་། 5. སྦྱིན་སྲེག་དང༌། 6. དཀྱིལ་འཁོར་བཞེངས་དང༌། 7. རབ་གནས། 8. གཏོར་མ་སྟེར། 9. སྔགས་བཟླས། 10. བརྟུལ་ཞུགས་དམ་ཚིག 11. སེམས་ཅན་བསྐྱངས། 12. སངས་རྒྱས་མཆོད་དང་། 13ཛམ་བྷ་ལར་ཆུ་སྦྱིན་དང་། 14. དགེ་ལས་ཚ་ཚ་འདེབས་པ་བཅུ་བཞིའོ།</t>
+          <t>གུར་ལས་དམ་ཚིག་བཅུ་བཞི་གསུངས་ཏེ། 1. དཀོན་མཆོག་མི་སྤང་། 2. དམ་ཚིག་རྟག་ཏུ་སྤྱད། 3. རྡོར་དྲིལ། 4. གཙུག་ཏོར་འཆང་དང་། 5. སྦྱིན་སྲེག་དང༌། 6. དཀྱིལ་འཁོར་བཞེངས་དང༌། 7. རབ་གནས། 8. གཏོར་མ་སྟེར། 9. སྔགས་བཟླས། 10. བརྟུལ་ཞུགས་དམ་ཚིག 11. སེམས་ཅན་བསྐྱངས། 12. སངས་རྒྱས་མཆོད་དང་། 13ཛམ་བྷ་ལ</t>
         </is>
       </c>
       <c r="C2015" s="1" t="inlineStr">
@@ -35020,7 +35020,7 @@
       </c>
       <c r="B2076" s="1" t="inlineStr">
         <is>
-          <t>གཟུགས་མི་སྡུག་པ། སྐྲ་བྱི་བ། དཔྲལ་བ་ཆུང་བ། མདོག་སེར་སྐྱ། མིག་སེར་པ། སྨིན་མཚམས་འབྱར་བ། སྣ་ལེབ་པ། སོ་སྟོར་བ། དིག་པ། མིག་ཟླུམ་པ། མིག་ཆུང་བ། ཕྱི་ནང་དུ་སྒུར་བ། ལྟོ་བ་ཆེ་བ། དཔུང་པ་དང་རྗེ་ངར་ཐུང་བ། སྤུ་ཅན། ལག་པ་དང་རྐང་པ་མི་མཉམ་པ། ཚིགས་སྦོམ་པ། ཁ་དང་ལུས་ལས་དྲི་ངན་པ་འབྱུང་བ་སྟེ་ལུས་ལ་མི་སྡུག་པའི་ཉེས་པའམ་སྐྱོན་བཅོ་བརྒྱད།</t>
+          <t>གཟུགས་མི་སྡུག་པ། སྐྲ་བྱི་བ། དཔྲལ་བ་ཆུང་བ། མདོག་སེར་སྐྱ། མིག་སེར་པ། སྨིན་མཚམས་འབྱར་བ། སྣ་ལེབ་པ། སོ་སྟོར་བ། དིག་པ། མིག་ཟླུམ་པ། མིག་ཆུང་བ། ཕྱི་ནང་དུ་སྒུར་བ། ལྟོ་བ་ཆེ་བ། དཔུང་པ་དང་རྗེ་ངར་ཐུང་བ། སྤུ་ཅན། ལག་པ་དང་རྐང་པ་མི་མཉམ་པ། ཚིགས་སྦོམ་པ། ཁ་དང་ལུས་ལས་དྲི་ངན་པ་འབྱུང་</t>
         </is>
       </c>
       <c r="C2076" s="1" t="inlineStr">
@@ -35457,7 +35457,7 @@
       </c>
       <c r="B2102" s="1" t="inlineStr">
         <is>
-          <t>དེ་ཡང་སངས་རྒྱས་འདས་ནས་ལོ་དགུ་བརྒྱ་ལྷག་སྟོང་དུ་ཉེ་བ་ན། སློབ་དཔོན་ཐོགས་མེད་ཀྱིས་མགོན་པོ་བྱམས་པ་བསྒྲུབ་ཏེ། བཀའ་ཐ་མ་དོན་རྣམ་པར་ངེས་(མདོ་སྡེ་ས་བཅུ་པ་ལ་སོགས་མི་ཡུལ་དུ་གདན་དྲངས་)པ་གཏན་ལ་འབབ་པར་མཛད་དེ། དེ་ཡང་མདོ་སྡེ་རྒྱན་དང་མངོན་རྟོགས་རྒྱན་གཉིས། དབུས་དང་མཐའ་རྣམ་འབྱེད་དང་། ཆོས་དང༌ཆོས་ཉིད་རྣམ་འབྱེད་གཉིས། ཐེག་པ་ཆེན་པོའི་རྒྱུད་བླ་མ་སྟེ། བྱམས་ཆོས་སྡེ་ལྔ་གསན་ནས་མི་ཡུལ་དུ་བྱོན་ཏེ་ཡི་གེར་བཀོད། ཐོགས་མེད་རང་གི་གཞི་བསྡུ་བ། རྣམ་གྲངས་བསྡུ་བ། རྣམ་པ་གཏན་ལ་འབབ་པ་བསྡུ་བ། རྣམ་པར་བཤད་པའི་སྒོ་བསྡུ་བ། ། རྩ་བ་ལྟ་བུའི་སའི་དངོས་གཞི་བསྡུ་བ་སྟེ། རྒྱས་པའི་བསྟན་བཅོས་ས་སྡེ་ལྔ་། ཐེག་པ་ཐུན་མོང་གི་ཆོས། མངོན་པ (འདི་མངོན་པ་གོང་མར་གྲགས）ཀུན་ལས་བཏུས་དང་། ཐེག་པ་ཆེན་པོའི་སྡོམ་ཐེག་བསྡུས་ཏེ། བསྡུས་པའི་བསྟན་བཅོས་སྡོམ་རྣམ་གཉིས་མཛད་དེ། ཐེག་པ་ཆེན་པོ་རྒྱ་ཆེན་སྤྱོད་པའི་སྲོལ་ཕྱེས་སོ། དེའི་གཅུང་སློབ་དཔོན་དབྱིག་གཉེན་གྱིས་ཁ་ཆེའི་སློབ་དཔོན་འདུས་བཟང་བརྟེན་ཏེ། ཡེ་ཤེས་འཇུག་པ་ལ་སོགས་མངོན་པ་སྡེ་བདུན་ལ་སོགས་གསན་སྐབས་སུ་གཅེན་ཐོགས་མེད་ལ། བྱམས་ཆོས་ལྔ། ས་སྡེ་ལྔ། སྡོམ་རྣམ་གཉིས་སོགས་གསན་ནས། དབྱིག་གཉེན་གྱིས་སེམས་ཙམ་པྲ་ཀ་ར་(པྲ་ཀ་ར་ནི་བོད་སྐད་དུ་རབ་ཏུ་བྱེད་པའོ།》སྡེ་བརྒྱད་མཛད་དེ། ཉི་ཤུ་པའི་རབ་ཏུ་བྱེད་པ་དང་། སུམ་ཅུ་པའི་རབ་ཏུ་བྱེད་པ། ཕུང་པོ་ལྔ་རབ་ཏུ་བྱེད་པ་དང༌། རྣམ་བཤད་རིག་པ། ལས་གྲུབ་པའི་རབ་ཏུ་བྱེད་པ་སྟེ་རང་རྒྱུད་དུ་བརྩམས་པ་ལྔ་དང༌། བརྟེན་འབྲེལ་མདོའི་འགྲེལ་བ། མདོ་སྡེ་རྒྱན་གྱི་འགྲེལ་བ། དབུས་མཐའི་འགྲེལ་བ་སྟེ། གཞན་འགྲེལ་དུ་བརྩམས་པ་གསུམ་སྟེ། རབ་ཏུ་འབྱེད་པའི་རྒྱུད་ (འདི་བརྒྱད་ཐོས་པ་དང་བཤད་པ་ལྟ་བུར་ལེན་གྱི་བསྟན་བཅོས། ) སྔར་གྱི་བཅུ་གཉིས་དང་བསྡོམས་པས་བྱམས་པ་འགྲེལ་བའི་ཆོས་ཉི་ཤུའོ། དེ་ནས་སློབ་དཔོན་དབྱིག་གཉེན་གྱིས་མངོན་པ་མཛོད་བརྩམས་ཏེ་མངོན་པར་འོག་པར་གྲགས་པའོ། སླར་ཡང་དེ་དག་གསལ་བར་བྱ་བའི་ཕྱིར་མངོན་པར་མཛོད་རང་འགྲེལ་ (འདི་བ་ཚབས་ལོ་ཙྰ་བ་ཉི་མ་གྲགས་ཀྱིས་བོད་དུ་སྒྱུར) དང་བཅས་པ་བརྩམས་པའོ།</t>
+          <t>དེ་ཡང་སངས་རྒྱས་འདས་ནས་ལོ་དགུ་བརྒྱ་ལྷག་སྟོང་དུ་ཉེ་བ་ན། སློབ་དཔོན་ཐོགས་མེད་ཀྱིས་མགོན་པོ་བྱམས་པ་བསྒྲུབ་ཏེ། བཀའ་ཐ་མ་དོན་རྣམ་པར་ངེས་(མདོ་སྡེ་ས་བཅུ་པ་ལ་སོགས་མི་ཡུལ་དུ་གདན་དྲངས་)པ་གཏན་ལ་འབབ་པར་མཛད་དེ། དེ་ཡང་མདོ་སྡེ་རྒྱན་དང་མངོན་རྟོགས་རྒྱན་གཉིས། དབུས་དང་མཐའ་རྣམ་འབྱེད་དང་། ཆོས་དང༌ཆོས་ཉིད་རྣམ་འབྱེད་གཉིས། ཐེག་པ་ཆེན་པོའི་རྒྱུད་བླ་མ་སྟེ། བྱམས་ཆོས་སྡེ་ལྔ་གསན་ནས་མི་ཡུལ་དུ་བྱོན་ཏེ་ཡི་གེར་བཀོད། ཐོགས་མེད་རང་གི་གཞི་བསྡུ་བ། རྣམ་གྲངས་བསྡུ་བ། རྣམ་པ་གཏན་ལ་འབབ་པ་བསྡུ་བ། རྣམ་པར་བཤད་པའི་སྒོ་བསྡུ་བ། ། རྩ་བ་ལྟ་བུའི་སའི་དངོས་གཞི་བསྡུ་བ་སྟེ། རྒྱས་པའི་བསྟན་བཅོས་ས་སྡེ་ལྔ་། ཐེག་པ་ཐུན་མོང་གི་ཆོས། མངོན་པ (འདི་མངོན་པ་གོང་མར་གྲགས）ཀུན་ལས་བཏུས་དང་། ཐེག་པ་ཆེན་པོའི་སྡོམ་ཐེག་བསྡུས་ཏེ། བསྡུས་པའི་བསྟན་བཅོས་སྡོམ་རྣམ་གཉིས་མཛད་དེ། ཐེག་པ་ཆེན་པོ་རྒྱ་ཆེན་སྤྱོད་པའི་སྲོལ་ཕྱེས་སོ། དེའི་གཅུང་སློབ་དཔོན་དབྱིག་གཉེན་གྱིས་ཁ་ཆེའི་སློབ་དཔོན་འདུས་བཟང་བརྟེན་ཏེ། ཡེ་ཤེས་འཇུག་པ་ལ་སོགས་མངོན་པ་སྡེ་བདུན་ལ་སོགས་གསན་སྐབས་སུ་གཅེན་ཐོགས་མེད་ལ། བྱམས་ཆོས་ལྔ། ས་སྡེ་ལྔ། སྡོམ་རྣམ་གཉིས་སོགས་གསན་ནས། དབྱིག་གཉེན་གྱིས་སེམས་ཙམ་པྲ་ཀ་ར་(པྲ་ཀ་ར་ནི་བོད་སྐད་དུ་རབ་ཏུ་བྱེད་པའོ།》སྡེ་བརྒྱད་མཛད་དེ། ཉི་ཤུ་པའི་རབ་ཏུ་བྱེད་པ་དང་། སུམ་ཅུ་པའི་རབ་ཏུ་བྱེད་པ། ཕུང་པོ་ལྔ་རབ་ཏུ་བྱེད་པ་དང༌། རྣམ་བཤད་རིག་པ། ལས་གྲུབ་པའི་རབ་ཏུ་བྱེད་པ་སྟེ་རང་རྒྱུད་དུ་བརྩམས་པ་ལྔ་དང༌། བརྟེན་འབྲེལ་མདོའི་འགྲེལ་བ། མདོ་སྡེ་རྒྱན་གྱི་འགྲེལ་བ། དབུས་མཐའི་འགྲེལ་བ་སྟེ། གཞན་འགྲེལ་དུ་བརྩམས་པ་གསུམ་སྟེ། རབ་ཏུ་འབྱེད་པའི་རྒྱུད་ (འདི་བརྒྱད་ཐོས་པ་དང་བཤད་པ་ལྟ་བུར་ལེན་གྱི་བསྟན་བཅོས། ) སྔར་གྱི་བཅུ་གཉིས་དང་བསྡོམས་པས་བྱམས་པ་འགྲེལ་བའི་ཆོས་ཉི་ཤུའོ། དེ་ནས་སློབ་དཔོན་དབྱིག་གཉེན་གྱིས་མངོན་པ་མཛོད་བརྩམས་ཏེ་མངོན་པར་འོག་པར་གྲགས་པའོ། སླར་ཡང་དེ་དག་གསལ་བར་བྱ་བའི་ཕྱིར་མངོན་པར་མཛོད་རང་འགྲེལ་ (འདི་བ་ཚབས་ལོ་ཙྰ་བ་ཉི་མ་གྲགས་ཀྱིས་བོད་དུ་སྒྱུར) ད</t>
         </is>
       </c>
       <c r="C2102" s="1" t="inlineStr">
@@ -35695,7 +35695,7 @@
       </c>
       <c r="B2116" s="1" t="inlineStr">
         <is>
-          <t>ཐང་རྒྱལ་རབས་ཀྱི་རྒྱས་ས་ནི་ཁྲང་ཨན(དེང་སང་ཧྲན་ཤིས་ཞིང་ཆེན་གྱི་ཤིས་ཨན）རྒྱལ་རབས་འདིར་སྔ་རྗེས་སུ་གོང་མ་མི་རབས་ཉི་ཤུ་རྩ་ལྔ་བྱུང(རུས་མིང་ནི་ལི་ཡིན）། 1. ཐང་ཀའོ་ཙུའུ་ལི་ཡུའན། 2. ཐང་ཐའི་ཙུང་ལི་ཧྲི་མིང་། 3. ཐང་ཀའོ་ཙུང་ལི་ཀྲི་4. ཐང་ཀྲུང་ཙུང་ལི་ཤིའན། 5. ཐང་རུའས་ཙུང་ལི་ཏན། 6. རྒྱལ་མོ་འུ་ཙེ་ཐེན། 7. ཐང་ཀྲུང་ཙུང་ལི་ཤིའན། 8. ཐང་ཧྲང་ཏི་ཁྲུང་མའོ། 9. ཐང་རུའས་ཙུང་ལི་ཏན། 10. ཐང་ཞོན་ཙུང་ལི་ལུང་ཅིས། 11. ཐང་སུད་ཙུང་ལི་ཧིང༌། 12. ཐང་ཏའི་ཙུང་ལི་ཡུས། 13. ཐང་ཏེ་ཙུང་ལི་ཞུའོ། 14. ཐང་ཧྲུན་ཙུང་ལི་སོང་། 15. ཐང་ཤན་ཙུང་ལི་ཁྲུན། 16. ཐང་མུའུ་ཙུང་ལི་ཧེང་། 17. ཐང་ཅིང་ཙུང་ལི་ཀྲེན། 18. ཐང་ཝེན་ཙུང་ལི་ཨང་། 19. ཐང་ཨུ་ཙུང་ལི་དབྱན། 20. ཐང་ཤོན་ཙུང་ལི་ཁྲེན། 21. ཐང་དབྱི་ཙུང་ལི་ཧོའི། 22. ཐང་ཤིས་ཙུང་ལི་ཞོན། 23. ཐང་ཀྲའོ་ཙུང་ལི་གཡི། 24. ཐང་ཨེད་རྟི་ལི་ཀྲུའུ་བཅས་ཀྱིས་སྤྱི་ལོ 618—907 བར་ལོ་ངོ་ཉིས་བརྒྱ་དགུ་བཅུ་བར་སྲིད་དབང་བཟུང་། ཐང་རྒྱལ་རབས་འགོ་ཚུགས་པ་དང་དུས་མཚུངས་སུ་བོད་ས་གནས་སུ་ཡང་རྒྱལ་པོ་སྲོང་བཙན་སྒམ་པོས་བོད་ས་གནས་ཚོ་པ་ཁ་གཅིག་གྱུར་བྱས་པའི་མི་རིགས་ཀྱི་སྲིད་དབང་ཐེངས་དང་པོར་བཙུགས་པ་ནས་བཟུང་རྒྱ་བོད་མི་རིགས་བར་གྱི་དཔལ་འབྱོར་དང་རིག་གནས་སྤེལ་རེས་ཀྱི་འབྲེལ་བ་གོང་འཕེལ་བྱུང་བའི་དུས་སྐབས་གསར་བ་ཞིག་གི་འགོ་ཚུགས་པ་དང་། ཐང་བོད་བར་ས་མཚམས་ཐོག་དམག་འཁྲུག་ཐེངས་མང་བྱུང་ཡང་དེས་ཐང་བོད་བར་གྱི་མཛའ་གྲོགས་འབྲེལ་བར་གནོད་སྐྱོན་ཆེན་པོ་གང་ཡང་བྱུང་མེད།</t>
+          <t>ཐང་རྒྱལ་རབས་ཀྱི་རྒྱས་ས་ནི་ཁྲང་ཨན(དེང་སང་ཧྲན་ཤིས་ཞིང་ཆེན་གྱི་ཤིས་ཨན）རྒྱལ་རབས་འདིར་སྔ་རྗེས་སུ་གོང་མ་མི་རབས་ཉི་ཤུ་རྩ་ལྔ་བྱུང(རུས་མིང་ནི་ལི་ཡིན）། 1. ཐང་ཀའོ་ཙུའུ་ལི་ཡུའན། 2. ཐང་ཐའི་ཙུང་ལི་ཧྲི་མིང་། 3. ཐང་ཀའོ་ཙུང་ལི་ཀྲི་4. ཐང་ཀྲུང་ཙུང་ལི་ཤིའན། 5. ཐང་རུའས་ཙུང་ལི་ཏན། 6. རྒྱལ་མོ་འུ་ཙེ་ཐེན། 7. ཐང་ཀྲུང་ཙུང་ལི་ཤིའན། 8. ཐང་ཧྲང་ཏི་ཁྲུང་མའོ། 9. ཐང་རུའས་ཙུང་ལི་ཏན། 10. ཐང་ཞོན་ཙུང་ལི་ལུང་ཅིས། 11. ཐང་སུད་ཙུང་ལི་ཧིང༌། 12. ཐང་ཏའི་ཙུང་ལི་ཡུས། 13. ཐང་ཏེ་ཙུང་ལི་ཞུའོ། 14. ཐང་ཧྲུན་ཙུང་ལི་སོང་། 15. ཐང་ཤན་ཙུང་ལི་ཁྲུན། 16. ཐང་མུའུ་ཙུང་ལི་ཧེང་། 17. ཐང་ཅིང་ཙུང་ལི་ཀྲེན། 18. ཐང་ཝེན་ཙུང་ལི་ཨང་། 19. ཐང་ཨུ་ཙུང་ལི་དབྱན། 20. ཐང་ཤོན་ཙུང་ལི་ཁྲེན། 21. ཐང་དབྱི་ཙུང་ལི་ཧོའི། 22. ཐང་ཤིས་ཙུང་ལི་ཞོན། 23. ཐང་ཀྲའོ་ཙུང་ལི་གཡི། 24. ཐང་ཨེད་རྟི་ལི་ཀྲུའུ་བཅས་ཀྱིས་སྤྱི་ལོ 618—907 བར་ལོ་ངོ་ཉིས་བརྒྱ་དགུ་བཅུ་བར་སྲིད་དབང་བཟུང་། ཐང་རྒྱལ་རབས་འགོ་ཚུགས་པ་དང་དུས་མཚུངས་སུ་བོད་ས་གན</t>
         </is>
       </c>
       <c r="C2116" s="1" t="inlineStr">
@@ -35746,7 +35746,7 @@
       </c>
       <c r="B2119" s="1" t="inlineStr">
         <is>
-          <t>དེ་ལ་ཡུལ་ཉེར་བཞི་ཡང་ཟེར། 1. པཱུ་ལི་ར་མ་ལ་ཡ (རྒྱ་གར་ཤར་ཕྱོགས་བྷང་གྷ་ལ་ཡི་ལྷོ་ངོས་མ་ལ་ཡའི་ཆུ་ཀླུང་འབབ་པའི་གནས་）།2. ཛ་ལནྡྷ་ར(ཆུ་བོ་གང་ག་མཚོ་མ་ཕམ་ནས་མངའ་རིས་ཀྱི་ཡུལ་བརྒྱུད་དེ་ཉིན་འགའ་ཞིག་ལྷོ་ནུབ་ཕྱོགས་སུ་ཁ་གཏད་ནས་འབབ་ཅིང་། ཌི་ལིའམ་ངྷི་ལིའི་བྱང་ཕྱོགས་ཧ་རི་དཱ་ཝར་ནས་ཤར་ཕྱོགས་སུ་འཁྱོགས་ནས་འབབ་པའི་བྱང་ངོ་། ཛ་ལ་མུག་གམ། ཛ་ལ་མུ་ཁི་སྟེ་རྡོ་ལ་མེ་འབར་པིའི་གནས)། 3.ˌཨཽ་ཊི་ཡ་ན (འདི་ཨོ་རྒྱན་གྱི་ཡུལ) 4. ཨ་རྦུ་ཏ (རྒྱ་གར་ལྷོ་ཕྱོགས་ཀྱི་རི་དབུས་མཐོ་ལ་མཐའ་དམའ་བ་འབྲང་རྒྱས་སམ་སྙིང་གི་གཟུགས་ཅན་ཞིག་གི་མིང་།）5. གོོ་ད་ཝ་རི་(བལ་པོའི་ཡུལ་གྱི་བྱང་ངོས་རང་རྒྱལ་གྱི་གཉའ་ནང་ཤན་གྱི་ཉེ་འདབས་ལ་ཕྱི་གངས་ར་ཞེས་གངས་རི་ཆེན་པོ་ཞིག་ཡོད་པར་བཤད་པ་ལྟར་ན། དེང་སང་གི་ས་བཀྲའི་ཐོག་ཏུ་སྒོ་ས་ཡིན་ཐན་རི་བོ་ཞེས་སམ། ཡོངས་གྲངས་སུ་ཤི་ཤ་སྦང་མའི་རི་བོ་ཞེས་པ་དེ་ཡིན་ནམ་སྙམ་བརྟག འདི་རྗེ་བཙུན་མི་ལའི་རྣམ་ཐར་དུ། སྟོད་གཉའ་ནང་དུ་ཡོད་པའི་ལ་ཕྱི་གངས་ར་ཞེས་གསལ་ཞིང་། ལ་ཕྱི་གངས་ར་ཞེས་པ་ཧི་མ་ལ་ཡའི་རི་ཡི་རྒྱུད་གཅིག་ཡིན་པས། ས་བཀྲའི་ནང་སྒོ་ས་ཡིན་ཐན་ཞེས་གསལ་ཞིང་། དེང་སང་ཡོངས་གྲགས་རྒྱ་སྐད་དུ་ཤི་ཤ་སྦང་མ་ཞེས་པ་དེ་ཡིན་ནམ། དེ་མིན་ལ་ཕྱི་གངས་ར་ཞེས་པ་ལོགས་སུ་ཡོད་མེད་བརྟག་དགོས། 6. རྭ་མེ་ཤ་རི་(རྒྱ་གར་གྱི་ས་དབྱིབས་གྲུ་གསུམ་དུ་ཆགས་པའི་རྩེ་མོ་རྣོ་ཤོས་ལྷོ་ཕྱོགས་སུ་གཏད་པའི་རྒྱ་མཚོའི་འགྲམ་གྱི་སྣེ་དེར་ཡོད། འདི་ནས་ཤར་ལྷོ་ཕྱོགས་སུ་གྲུ་བཏང་ནས་སོང་ན་ལང་ཀའི་གྲོང་ཁྱེར་རམ་ལམ་ཀའི་གླིང་ཕྲན་ཞེས་རྒྱལ་པོ་ར་མཱ་ནས་སྲིན་ཡུལ་དུ་དམག་དྲངས་པར་བཤད་པའི་ཡུལ་དེ་ཡིན་པས། དེང་སང་སིང་ག་ལའང་ཤྲི་ལངྐའམ་སི་ལི་ལངྐ་ཟེར། ）7. དེ་ཝི་ཀོ་ཏྲི། འདི་བོད་སྐད་དུ་ལྷ་མོའི་མཁར་ཞེས་ཟེར་ཞིང་འདི་ལ་ངོས་འཛིན་ཚུལ་མི་འདྲ་བ་གཉིས་ཏེ། ཀོང་པོའི་ཡུལ་དང་དྭགས་པོ། ཀློ་ཡུལ་གསུམ་གྱི་འཚམས་ཡོད་པའི་རྩ་རི་ལ་ངོས་འཛིན་པ་གཅིག་དང་། རྒྱ་གར་ཨ་སམ་གྱི་ཤར་ཕྱོགས། གང་ཚ་རངྒ་ཞེས་པའི་ནང་ཚང་ཏི་ར་ཕུར་ཞེས་པའི་རི་བོ་དེར་ངོས་འཛིན་པ་གཅིག་ཡོད། 8. མཱ་ལ་ཝ (རྒྱ་གར་ནུབ་ཕྱོགས་རྒྱ་མཚོའི་གླིང་ཕྲན་ཞིག་ཡིན་པར་བཤད། ）9. ཀ་མ་རུ་པ (བལ་ཡུལ་དང་ཐག་ཉེ་བའི་གངས་རྒྱལ་མོ་མཐོན་མཐིང་གི་འགྲམ་ནས &lt;རྒྱ་གར་སྐད་དུ་ཆུ་བོ་ལོ་ཧི་ཏ་རྒྱ་སྐད་དུ་མཱ་མཆོན་ཧཱོ&gt; བོད་སྐད་དུ་རྟ་མཆོག་ཁ་འབབ་ཏུ་གྲགས་པ་དེ་ཉིད་གཞིས་ཀ་རྩེ་ནས་ཉང་ཆུ་དང་འདྲེས། ལྷ་སའི་ལྷོ་ནུབ་ཆུ་ཤུལ་ནས་སྐྱིད་ཆུ་དང་འདྲེས་ནས་ཡར་ལུང་བརྒྱུད་དུ་འབབ་པ་ལ་ཡར་ལུང་གཙང་པོ་ཟེར། དེ་ཉིད་ཀོང་པོ་ཡུལ་ནས་ཁ་ལྷོར་བལྟས་ནས་རྒྱ་གར་ཤར་ཕྱོགས་སུ་ཐོན་པའི་ས་དེར་ངོས་འཛིན། དེ་ནས་རྒྱ་གར་ཤར་ཕྱོགས་ཨ་སམ་གྱི་ཡུལ་བརྒྱུད་ནས་ཤར་པ་ཀི་སི་ཐན་གྱི་བྱང་ནས་ཁ་ལྷོར་བལྟས་ནས་རྒྱ་མཚོ་ཆེན་པོར་འབབ་པས་གོང་གསལ་ཆུ་བོའི་དེའི་དུམ་བུ་ལ་རྒྱ་གར་བ་རྣམས་ཀྱིས་བྷ་རམ་པུརྡ་ཟེར། ）10. ཨོ་ཏྲི(རྒྱ་གར་ལྷོ་ཕྱོགས་རྒྱལ་པོ་ཤིང་རྟ་བཅུ་པའི་ཡུལ་ལ་ངོས་འཛིན་པར་བཤད་ཀྱང་ས་གནས་ངོས་མ་ཟིན།）11. ཏྲི་ཤ་ཀུ་ནི (རྒྱ་གར་ནུབ་ཕྱོགས་ཆུ་བོ་གངྒ་དང་། གན་ཏི་སུ་རུ་པ་གསུམ་གྱི་འདུས་མདོ་དེར་ཡོད།）12. ཀོ་ས་ལ་(རྒྱ་གར་ཡུལ་དབུས་གཉན་ཡོད་ཅེས་པ་དེ་ཡིན།）13. ཀལིངྐ (རྒྱ་གར་ལྷོ་ཕྱོགས་རྒྱ་མཚོའི་འགྲམ་གྱི་ཡུལ་ལ་ཏྲིལིངྐ་ལ་སོགས་པའི་ལིངྒའི་མིང་ཅན་བརྒྱད་ཙམ་ཡོད་པར་བཤད་པའི་ནང་ནས་གཅིག་ཡིན། ）14. ལམ་པ་ཀ (ཨོ་རྒྱན་གྱི་ཡུལ་གྱི་ཤར་ཕྱོགས་སུ་ཡོད་པར་བཤད།）15. ཀཉྩི (རྒྱ་གར་ལྷོ་ཕྱོགས་ཀྱི་དཀྱིལ་ཏྲི་ལིང་ཀ་ཞེས་པ་དེ་ཡིན་པར་བཤད། ）16. ཧི་མ་ལ་ཡ། བོད་སྐད་དུ་རི་བོ་གངས་ཅན་ཞེས་རྒྱ་གར་གྱི་བྱང་ཕྱོགས་སུ་ཡོད་པའི་རི་རྒྱུད་ཤིན་ཏུ་རིང་བ་ཞིག་གི་མིང་། 17. སྦེ་ཏ (མངའ་རིས་གུ་གེའི་ཡུལ་དུ་ཡོད།）18. གྲི་ཧ་དེ་ཝ་ཏ(ལི་ཡུལ་ལྕང་ར་སྨུག་པོའམ། དེང་སང་ཤིན་ཅང་དུ་འབོད་པའི་གནས་ཀྱི་ནུབ་ངོས་སུ་ཡོད་པར་བཤད།）19. སོ་ར་ཥྟྲ(འདི་བོད་སྐད་དུ་བཟང་པོ་ཅན་ཟེར་ཞིང་རྒྱ་གར་ནུབ་ཕྱོགས་ཀྱི་ཡུལ་ཞིག་ཡིན་པར་བཤད་པ་ལྟར་རང་རྒྱལ་ནས་པར་བསྐྲུན་བྱས་པའི་ས་བཀྲའི་ནང་དུ་རྒྱ་གར་ནུབ་ཕྱོགས་རྒྱ་མཚོའི་འགྲམ་གྱི་ཡུལ་ཞིག་ལ་སུ་ལ་ཐའོ་ཞེས་འཁོད་པ་དེ་ཡིན་སྙམ།）20. སུ་ཝརྣ་དཱི་པ（འདི་བོད་སྐད་དུ་གསེར་གླིང་ཟེར་ཞིང་། དེང་སང་ཨེན་རྡུ་ཉི་ཤི་ཡའི་རྒྱལ་ས་ཡ་ཙཱ་ཏཱ་ཡི་ནུབ་བྱང་ངོས་ཀྱི་གླིང་ཕྲན་ཆེ་བ་སུ་མན་ཏ་ལ་ཟེར་བ་དེ་ཡིན་ཞེ་ས་རྒྱ་རིགས་ཀྱི་མཁས་པའི་དབང་པོ་འགའ་ཞིག་གིས་གསུངས་པ་ཐོས།）21. ནཱ་ཀ་ར (རྒྱ་གར་བྱང་ཕྱོགས་བལ་ཡུལ་དང་ཁད་ཉེ་བར་ཆུ་བོ་གངྒཱའི་འགྲམ་དུ་གྲོང་ཁྱེར་པ་པ་ཏྲ་ལི་བུ་ཏྲ་འམ (བོད་སྐད་དུ་སྐྱ་བོའི་བུ་ཟེར）པ་ཋན་ཞེས་ནཱ་ག་རའི་ཡི་གེ་འབྱུང་བའི་ཡུལ་དེ་ཡིན་པར་བཤད། ）22. སིན་དྷུ། གངས་རི་ཏི་སེའི་བྱང་ངོས་ནས་འབབ་པའི་ཆུ་བོ་སིན་དྷུ་ཞེས་པ། བོད་སྐད་དུ་སེངྒེ་ཁ་འབབ་ཟེར། དེ་མངའ་རིས་ཀྱི་ཡུལ་བརྒྱུད་དང་པོར་བྱང་དང་། དེ་ནས་པ་ལི་ཅ་སིའི་ལྷོ་ངོས་ནས་རེ་ཞིག་བར་ནུབ་དྲང་པོ་དང་དེ་ནས་ཀསྨིརའམ། ཁ་ཧྲི་སྨིར་གྱི་ཤར་ངོས་ནས་ནུབ་བྱང་བར་འཁྱོག་ནས་འབབ་ཅིང་། མཐར་ནུབ་པ་ཀི་སི་ཐན་གྱི་བྱང་ཤར་ནས་དཀྱིལ་དྲང་པོ་བརྒྱུད་རྒྱལ་ས་ཁ་ར་ཏྲིའམ་སྔ་དུས་ཁ་ར་ཋར་འབོད་པའི་ཉེ་འདབས་ནས་ཨ་ར་པིའི་རྒྱ་མཚོར་འབབ་པས། རྒྱལ་སའི་ཉེ་འདབས་སུ་གོང་གི་གནས་དེ་ཡོད་པར་བཤད། 23. མ་རུ། ཀསྨིར་གྱི་བྱང་ཕྱོགས་ཛ་ལནྡྷ་ར་འི་ཉེ་འདབས་སུ་ཡོད་པར་བཤད། 24. ཀུ་ལུ་ཏ། ཀསྨིར་གྱི་བྱང་ཕྱོགས་ཀྱི་མཐའ་མཚམས་མངའ་རིས་ཀྱི་ཡུལ་དང་ཐག་ཉེ་བར་ཡོད་པ་དང་། མངའ་རིས་པ་རྣམས་ཀྱིས་ཉུང་རྡའི་ཡུལ་ཞེས་འབོད་པའི་ནང་ཚན་ཞིག་ཡིན་པར་བཤད།</t>
+          <t>དེ་ལ་ཡུལ་ཉེར་བཞི་ཡང་ཟེར། 1. པཱུ་ལི་ར་མ་ལ་ཡ (རྒྱ་གར་ཤར་ཕྱོགས་བྷང་གྷ་ལ་ཡི་ལྷོ་ངོས་མ་ལ་ཡའི་ཆུ་ཀླུང་འབབ་པའི་གནས་）།2. ཛ་ལནྡྷ་ར(ཆུ་བོ་གང་ག་མཚོ་མ་ཕམ་ནས་མངའ་རིས་ཀྱི་ཡུལ་བརྒྱུད་དེ་ཉིན་འགའ་ཞིག་ལྷོ་ནུབ་ཕྱོགས་སུ་ཁ་གཏད་ནས་འབབ་ཅིང་། ཌི་ལིའམ་ངྷི་ལིའི་བྱང་ཕྱོགས་ཧ་རི་དཱ་ཝར་ནས་ཤར་ཕྱོགས་སུ་འཁྱོགས་ནས་འབབ་པའི་བྱང་ངོ་། ཛ་ལ་མུག་གམ། ཛ་ལ་མུ་ཁི་སྟེ་རྡོ་ལ་མེ་འབར་པིའི་གནས)། 3.ˌཨཽ་ཊི་ཡ་ན (འདི་ཨོ་རྒྱན་གྱི་ཡུལ) 4. ཨ་རྦུ་ཏ (རྒྱ་གར་ལྷོ་ཕྱོགས་ཀྱི་རི་དབུས་མཐོ་ལ་མཐའ་དམའ་བ་འབྲང་རྒྱས་སམ་སྙིང་གི་གཟུགས་ཅན་ཞིག་གི་མིང་།）5. གོོ་ད་ཝ་རི་(བལ་པོའི་ཡུལ་གྱི་བྱང་ངོས་རང་རྒྱལ་གྱི་གཉའ་ནང་ཤན་གྱི་ཉེ་འདབས་ལ་ཕྱི་གངས་ར་ཞེས་གངས་རི་ཆེན་པོ་ཞིག་ཡོད་པར་བཤད་པ་ལྟར་ན། དེང་སང་གི་ས་བཀྲའི་ཐོག་ཏུ་སྒོ་ས་ཡིན་ཐན་རི་བོ་ཞེས་སམ། ཡོངས་གྲངས་སུ་ཤི་ཤ་སྦང་མའི་རི་བོ་ཞེས་པ་དེ་ཡིན་ནམ་སྙམ་བརྟག འདི་རྗེ་བཙུན་མི་ལའི་རྣམ་ཐར་དུ། སྟོད་གཉའ་ནང་དུ་ཡོད་པའི་ལ་ཕྱི་གངས་ར་ཞེས་གསལ་ཞིང་། ལ་ཕྱི་གངས་ར་ཞེས་པ་ཧི་མ་ལ་ཡའི་རི་ཡི་རྒྱུད་གཅིག་ཡིན་པས། ས་བཀྲའི་ནང་སྒོ་ས་ཡིན་ཐན་ཞེས་གསལ་ཞིང་། དེང་སང་ཡོངས་གྲགས་རྒྱ་སྐད་དུ་ཤི་ཤ་སྦང་མ་ཞེས་པ་དེ་ཡིན་ནམ། དེ་མིན་ལ་ཕྱི་གངས་ར་ཞེས་པ་ལོགས་སུ་ཡོད་མེད་བརྟག་དགོས། 6. རྭ་མེ་ཤ་རི་(རྒྱ་གར་གྱི་ས་དབྱིབས་གྲུ་གསུམ་དུ་ཆགས་པའི་རྩེ་མོ་རྣོ་ཤོས་ལྷོ་ཕྱོགས་སུ་གཏད་པའི་རྒྱ་མཚོའི་འགྲམ་གྱི་སྣེ་དེར་ཡོད། འདི་ནས་ཤར་ལྷོ་ཕྱོགས་སུ་གྲུ་བཏང་ནས་སོང་ན་ལང་ཀའི་གྲོང་ཁྱེར་རམ་ལམ་ཀའི་གླིང་ཕྲན་ཞེས་རྒྱལ་པོ་ར་མཱ་ནས་སྲིན་ཡུལ་དུ་དམག་དྲངས་པར་བཤད་པའི་ཡུལ་དེ་ཡིན་པས། དེང་སང་སིང་ག་ལའང་ཤྲི་ལངྐའམ་སི་ལི་ལངྐ་ཟེར། ）7. དེ་ཝི་ཀོ་ཏྲི། འདི་བོད་སྐད་དུ་ལྷ་མོའི་མཁར་ཞེས་ཟེར་ཞིང་འདི་ལ་ངོས་འཛིན་ཚུལ་མི་འདྲ་བ་གཉིས་ཏེ། ཀོང་པོའི་ཡུལ་དང་དྭགས་པོ། ཀློ་ཡུལ་གསུམ་གྱི་འཚམས་ཡོད་པའི་རྩ་རི་ལ་ངོས་འཛིན་པ་གཅིག་དང་། རྒྱ་གར་ཨ་སམ་གྱི་ཤར་ཕྱོགས། གང་ཚ་རངྒ་ཞེས་པའི་ནང་ཚང་ཏི་ར་ཕུར་ཞེས་པའི་རི་བོ་དེར་ངོས་འཛིན་པ་གཅིག་ཡོད། 8. མཱ་ལ་ཝ (རྒྱ་གར་ནུབ་ཕྱོགས་རྒྱ་མཚོའི་གླིང་ཕྲན་ཞིག་ཡིན་པར་བཤད། ）9. ཀ་མ་རུ་པ (བལ་ཡུལ་དང་ཐག་ཉེ་བའི་གངས་རྒྱལ་མོ་མཐོན་མཐིང་གི་འགྲམ་ནས &lt;རྒྱ་གར་སྐད་དུ་ཆུ་བོ་ལོ་ཧི་ཏ་རྒྱ་སྐད་དུ་མཱ་མཆོན་ཧཱོ&gt; བོད་སྐད་དུ་རྟ་མཆོག་ཁ་འབབ་ཏུ་གྲགས་པ་དེ་ཉིད་གཞིས་ཀ་རྩེ་ནས་ཉང་ཆུ་དང་འདྲེས། ལྷ་སའི་ལྷོ་ནུབ་ཆུ་ཤུལ་ནས་སྐྱིད་ཆུ་དང་འདྲེས་ནས་ཡར་ལུང་བརྒྱུད་དུ་འབབ་པ་ལ་ཡར་ལུང་གཙང་པོ་ཟེར། དེ་ཉིད་ཀོང་པོ་ཡུལ་ནས་ཁ་ལྷོར་བལྟས་ནས་རྒྱ་གར་ཤར་ཕྱོགས་སུ་ཐོན་པའི་ས་དེར་ངོས་འཛིན། དེ་ནས་རྒྱ་གར་ཤར་ཕྱོགས་ཨ་སམ་གྱི་ཡུལ་བརྒྱུད་ནས་ཤར་པ་ཀི་སི་ཐན་གྱི་བྱང་ནས་ཁ་ལྷོར་བལྟས་ནས་རྒྱ་མཚོ་ཆེན་པོར་འབབ་པས་གོང་གསལ་ཆུ་བོའི་དེའི་དུམ་བུ་ལ་རྒྱ་གར་བ་རྣམས་ཀྱིས་བྷ་རམ་པུརྡ་ཟེར། ）10. ཨོ་ཏྲི(རྒྱ་གར་ལྷོ་ཕྱོགས་རྒྱལ་</t>
         </is>
       </c>
       <c r="C2119" s="1" t="inlineStr">
@@ -36273,7 +36273,7 @@
       </c>
       <c r="B2150" s="1" t="inlineStr">
         <is>
-          <t>1. ཆོས་ཐམས་ཅད་ནི་བདག་མེད་པ་ཡིན་ལ་སེམས་ཅན་རྣམས་བདག་མེད་པ་ལ་མ་མོས་པས་དེའི་ཕྱིར་སེམས་ཅན་རྣམས་ལ་དེ་བཞིན་གཤེཊ་པའི་ཐུགས་རྗེ་ཆེན་པོ་སྐྱེའོ། 2. ཆོས་ཐམས་ཅད་ནི་སེམས་ཅན་མེད་པ། 3. ཆོས་ཐམས་ཅད་ནི་སྲོག་མེད་པ། 4. ཆོས་ཐམས་ཅད་ནི་གང་ཟག་མེད་པ། 5. ཆོས་ཐམས་ཅད་ནི་རང་བཞིན་མེད་པ། 6. ཆོས་ཐམས་ཅད་ནི་གཞི་མེད་པ། 7. ཆོས་ཐམས་ཅད་ནི་གནས་མེད་པ། 8. ཆོས་ཐམས་ཅད་ནི་ང་ཡིར་བྱར་མེད་པ། 9. ཆོས་ཐམས་ཅད་ནི་བདག་པོ་མེད་པ། 10. ཆོས་ཐམས་ཅད་ནི་དངོས་པོ་མེད་པ། 11. ཆོས་ཐམས་ཅད་ནི་མ་སྐྱེས་པ། 12. ཆོས་ཐམས་ཅད་ནི་འཆི་འཕོ་བ་མེད་ཅིང་མི་སྐྱེས་པ། 13. ཆོས་ཐམས་ཅད་ནི་ཀུན་ནས་ཉོན་མོངས་པ་ཅན་མ་ཡིན་པ། 14. ཆོས་ཐམས་ཅད་ནི་འདོད་ཆགས་དང་བྲལ་བ། 15. ཆོས་ཐམས་ཅད་ནི་ཞེ་སྡང་དང་བྲལ་བ། 16. ཆོས་ཐམས་ཅད་ནི་གཏི་མུག་དང་བྲལ་བ། 17. ཆོས་ཐམས་ཅད་ནི་འོང་བ་མེད་པ། 18. ཆོས་ཐམས་ཅད་ནི་འགྲོ་བ་མེད་པ། 19. ཆོས་ཐམས་ཅད་ནི་མངོན་པར་འདུ་བྱེད་པ་མེད་པ། 20. ཆོས་ཐམས་ཅད་ནི་སྤྲོས་པ་མེད་པ། 21. ཆོས་ཐམས་ཅད་ནི་སྟོང་བ། 22. ཆོས་ཐམས་ཅད་ནི་མཚན་མ་མེད་པ། 23. ཆོས་ཐམས་ཅད་ནི་སྨོན་པ་མེད་པ། 24. ཀྱེ་མ་འཇིག་རྟེན་གནས་པ་འདི་ནི་ཕན་ཚུན་རྩོད་པས་ཡོངས་སུ་ཟིན་ཅིང་གནོད་སེམས་ཀྱིས་འཐབ་པ་དང་ཞེ་སྡང་ལ་ཞུགས་པར་གཟིགས། 25. ཀྱེ་མ་འཇིག་རྟེན་གནས་པ་འདི་ནི་ཕྱིན་ཅི་ལོག་དང་ལྡན་ཞིང་ལམ་ཉམ་ང་བར་ཞུགས་པ་ལམ་གོལ་བ་ལ་གནས་པ། 26. ཀྱེ་མ་འཇིག་རྟེན་གནས་པ་འདི་ནི་སྙམ་ཞིང་འདོད་པས་ཟིལ་གྱིས་ནོན་པ་སྟེ་ཆོག་མི་ཤེས་ཤིང་གཞན་གྱི་ནོར་ལ་འཕྲོག་པ། 27. ཀྱེ་མ་སེམས་ཅན་འདི་རྣམས་ནི་ནོར་དང་འབྲུ་དང་ཁྱིམ་དང་བུ་དང་ཆུང་མ་ལ་སྲེད་པས་འཁོར་བ་སྟེ་སྙིང་བོ་མེད་པ་ལ་སྙིང་བོར་འདུ་ཤེས་པ། 28. ཀྱེ་མ་སེམས་ཅན་འདི་དག་ནི་མ་རིག་པས་འཚོ་བ་སྟེ་གཅིག་ལ་གཅིག་འབྲིད་པར་གནས་པ། 29. ཀྱེ་མ་སེམས་ཅན་འདི་དག་ནི་ཆོག་མི་ཤེས་པ་སྟེ་རྙེད་པ་དང་བཀུར་སྟི་དང་ཚིགས་སུ་བཅད་པ་ལ་སྤྱོད་ཀྱང་བདག་ཅག་ནི་ཆོག་ཤེས་པའོ་སྙམ་དུ་འཛིན་པ། 30. ཀྱེ་མ་སེམས་ཅན་འདི་དག་ནི་ཁྱིམ་གྱི་གནས་ནས་སྡུག་བསྔལ་གྱི་སྣོད་ཀུན་ནས་ཉོན་མོངས་པ་ཅན་རྟག་ཏུ་དགའ་བ། 31. ཆོས་ཐམས་ཅད་ནི་རྒྱུས་ཉེ་བར་འགྲོ་བ་སྟེ་བསྒྲུབས་པས་ཉེ་བར་གནས་པའི་མཚན་ཉིད། 32. སེམས་ཅན་རྣམས་ནི་ཆགས་པ་མེད་པའི་ཡེ་ཤེས་དམ་པ་ཁྱད་པར་དུ་འཕགས་པ་ཡོངས་སུ་མྱ་ངན་ལས་འདས་པའི་འདི་བཏབ་ཞིང་གང་འདི་ཉན་ཐོས་ཀྱི་ཐེག་པ་དང་རང་སངས་རྒྱས་ཀྱི་ཐེག་པ་དམན་པ་ཚོལ་བ་ཡིན་གྱི་དེ་དག་ལ་གང་འདི་སངས་རྒྱས་ཡེ་ཤེས་ལ་དམིགས་པར་བྱ་བའི་ཕྱིར་རྒྱ་ཆེན་པོ་ལ་བློས་མོས་པར་བྱའམ་ཞེས་སེམས་ཅན་རྣམས་ལ་དེ་བཞིན་གཤེགས་པའི་ཐུགས་རྗེ་ཆེན་པོ་སྐྱེའོ།</t>
+          <t>1. ཆོས་ཐམས་ཅད་ནི་བདག་མེད་པ་ཡིན་ལ་སེམས་ཅན་རྣམས་བདག་མེད་པ་ལ་མ་མོས་པས་དེའི་ཕྱིར་སེམས་ཅན་རྣམས་ལ་དེ་བཞིན་གཤེཊ་པའི་ཐུགས་རྗེ་ཆེན་པོ་སྐྱེའོ། 2. ཆོས་ཐམས་ཅད་ནི་སེམས་ཅན་མེད་པ། 3. ཆོས་ཐམས་ཅད་ནི་སྲོག་མེད་པ། 4. ཆོས་ཐམས་ཅད་ནི་གང་ཟག་མེད་པ། 5. ཆོས་ཐམས་ཅད་ནི་རང་བཞིན་མེད་པ། 6. ཆོས་ཐམས་ཅད་ནི་གཞི་མེད་པ། 7. ཆོས་ཐམས་ཅད་ནི་གནས་མེད་པ། 8. ཆོས་ཐམས་ཅད་ནི་ང་ཡིར་བྱར་མེད་པ། 9. ཆོས་ཐམས་ཅད་ནི་བདག་པོ་མེད་པ། 10. ཆོས་ཐམས་ཅད་ནི་དངོས་པོ་མེད་པ། 11. ཆོས་ཐམས་ཅད་ནི་མ་སྐྱེས་པ། 12. ཆོས་ཐམས་ཅད་ནི་འཆི་འཕོ་བ་མེད་ཅིང་མི་སྐྱེས་པ། 13. ཆོས་ཐམས་ཅད་ནི་ཀུན་ནས་ཉོན་མོངས་པ་ཅན་མ་ཡིན་པ། 14. ཆོས་ཐམས་ཅད་ནི་འདོད་ཆགས་དང་བྲལ་བ། 15. ཆོས་ཐམས་ཅད་ནི་ཞེ་སྡང་དང་བྲལ་བ། 16. ཆོས་ཐམས་ཅད་ནི་གཏི་མུག་དང་བྲལ་བ། 17. ཆོས་ཐམས་ཅད་ནི་འོང་བ་མེད་པ། 18. ཆོས་ཐམས་ཅད་ནི་འགྲོ་བ་མེད་པ། 19. ཆོས་ཐམས་ཅད་ནི་མངོན་པར་འདུ་བྱེད་པ་མེད་པ། 20. ཆོས་ཐམས་ཅད་ནི་སྤྲོས་པ་མེད་པ། 21. ཆོས་ཐམས་ཅད་ནི་སྟོང་བ། 22. ཆོས་ཐམས་ཅད་ནི་མཚན་མ་མེད་པ། 23. ཆོས་ཐམས་ཅད་ནི་སྨོན་པ་མེད་པ། 24. ཀྱེ་མ་འཇིག་རྟེན་གནས་པ་འདི་ནི་ཕན་ཚུན་རྩོད་པས་ཡོངས་སུ་ཟིན་ཅིང་གནོད་སེམས་ཀྱིས་འཐབ་པ་དང་ཞེ་སྡང་ལ་ཞུགས་པར་གཟིགས། 25. ཀྱེ་མ་འཇིག་རྟེན་གནས་པ་འདི་ནི་ཕྱིན་ཅི་ལོག་དང་ལྡན་ཞིང་ལམ་ཉམ་ང་བར་ཞུགས་པ་ལམ་གོལ་བ་ལ་གནས་པ། 26. ཀྱེ་མ་འཇིག་རྟེན་གནས་པ་འདི་ནི་སྙམ་ཞིང་འདོད་པས་ཟིལ་གྱིས་ནོན་པ་སྟེ་ཆོག་མི་ཤེས་ཤིང་གཞན་གྱི་ནོར་ལ་འཕྲོག་པ། 27. ཀྱེ་མ་སེམས་ཅན་འདི་རྣམས་ནི་ནོར་དང་འབྲུ་དང་ཁྱིམ་དང་བུ་དང་ཆུང་མ་ལ་སྲེད་པས་འཁོར་བ་སྟེ་སྙིང་བོ་མེད་པ་ལ་སྙིང་བོར་འདུ་ཤེས་པ། 28. ཀྱེ་མ་སེམས་ཅན་འདི་དག་ནི་མ་རིག་པས་འཚོ་བ་སྟེ་གཅིག་ལ་གཅིག་འབྲིད་པར་གནས་པ། 29. ཀྱེ་མ་སེམས་ཅན་འདི་དག་ནི་ཆོག་མི་ཤེས་པ་སྟེ་རྙེད་པ་དང་བཀུར་སྟི་དང་ཚིགས་སུ་བཅད་པ་ལ་སྤྱོད་ཀྱང་བདག་ཅག་ནི་ཆོག་ཤེས་པའོ་སྙམ་དུ་འཛིན་པ། 30. ཀྱེ་མ་སེམས་ཅན་འདི་དག་ནི་ཁྱིམ་གྱི་གནས་ནས་སྡུག་བསྔལ་གྱི་སྣོད་ཀུན་ནས་ཉོན་མོངས་པ་ཅན་རྟག་ཏུ་དགའ་བ། 31. ཆོས་ཐམས་ཅད་ནི་རྒྱུས་ཉེ་བར་འགྲོ་བ་སྟེ་བསྒྲུབས་པས་ཉེ་བར་གནས་པའི་མཚན་ཉིད། 32. སེམས་ཅན་རྣམས་ནི་ཆགས་པ་མེད་པའི་ཡེ་ཤེས་དམ་པ་ཁྱད་པར་དུ་འཕགས་པ་ཡོངས་སུ་</t>
         </is>
       </c>
       <c r="C2150" s="1" t="inlineStr">
@@ -36341,7 +36341,7 @@
       </c>
       <c r="B2154" s="1" t="inlineStr">
         <is>
-          <t>1. སྔོན་བླ་མ་རྣམས་ལ་བསྐྱལ་བ་དང་བསུ་བ་སོགས་བྱས་པས་ཕྱག་དང་ཞབས་འཁོར་ལོའི་རྩིབས་སྟོང་མུ་ཁྱུད་བཅས་པ་རྫོགས་པ་དང༌། 2. སྡོན་སྡོམ་པ་ཡང་དག་པར་བླངས་པ་བརྟན་པོར་བསྲུང་བས། ཞབས་རུས་སྦལ་བཞིན་དུ་མཉམ་པ། 3. སྔོན་བསྡུ་དངོས་བཞི་བརྟེན་པར་བྱས་པས་ཕྱག་དང་ཞབས་ཀྱི་སོར་མོ་ངང་པའི་རྒྱལ་པོ་ལྟ་བུར་རིན་པོ་ཆེའི་དྲ་བས་འབྲེལ་བ། 4. སྔོན་བཟའ་བ་དང་བཅའ་བ་བྱིན་པས། ཕྱག་དང་ཞབས་ཤིང་བལ་ལྟར་འཇམ་ཞིང་གཞོན་ཤ་ཆགས་པ། 5. བདུན་མཐོ་བ་ནི་ཕྱག་གི་བོལ་གཉིས། ཞབས་ཀྱི་བོལ་གཉིས་དཔུང་མགོ་གཉིས། ལྟག་པའི་ཕྱོགས་མཐོ་བའོ། 6. སོར་མོ་རིང་བ་ནི་ཞབས་མཐིལ་གྱི་དཀྱུས་དང་མཐོ་མཉམ་པའོ། 7. རྟིང་པ་ཡངས་པ་ནི་ཞབས་ཀྱི་བཞི་ཆ་ཕྱིར་འཕགས་པའོ། 8. སྟོན་པའི་སྐུའི་མཐོ་དམན་ནི། འཛམ་བུ་གླིང་པའི་ཁྲུ་ཕྱེད་དང་བཅུ་གཅིག་ཡོད་དོ། འཛམ་བུ་གླིང་པའི་མི་ལས་ཁྲུ་བདུན་ལྷག་པས་ན་སྐུ་ཆེ་ཞིང་དྲང་བའོ། 9. ཞབས་ཀྱི་ལོང་བུ་འབུར་བ་ཕྱིར་མི་མངོན་པའོ། 10. སྐུའི་སྤུ་གྱེན་དུ་འཁྱིལ་ཞིང་གཡས་སུ་ཕྱོགས་པ་དང་། 11. བྱིན་པ་རི་དྭགས་ཨེ་ན་ཡའི་ལྟ་བུ་ནི་ཡོངས་སུ་མཉམ་ཞིང་རིམ་པར་མཚམས་ལ་རྒྱས་ཤིང་བལྟམས་པའོ། 12.ཕྱག་རིང་བ་ནི། མ་བཅུད་པར་ཕྱག་གིས་པུས་མོའི་སླ་ངར་སླེབས་པའོ། 13. འདོམས་ཀྱི་སྦ་བ་སྦུབས་སུ་ནུབ་པ་ནི། གླང་པོ་ཆེའི་ལྟ་བུའོ། 14. གསེར་གྱི་མདངས་ལྟར་ཤིན་ཏུ་དྭངས་པའོ། 15. ལྤགས་པ་འཇམ་པ་ནི་གསེར་སྦྱངས་པ་ལྟར་སྙོམས་ལ་རྡུལ་གྱིས་མི་གོས་པའོ། 16. བ་སྤུའི་བུ་ག་གཅིག་ལ་གཉིས་མེད་པར་དོར་ན་གཡས་སུ་ལེགས་པར་འཁྲུངས་པ་དང་། 17. མཛོད་སྤུ་ནི་སྨིན་མཚམས་སུ་ས་དཀར་འཇམ་གཡས་སུ་འཁྱིལ་བ་ཉི་ཟླ་ལས་ལྷག་པའི་འོད་དང་ལྡན་པའོ། 18. སྐུའི་རོ་སྟོད་འཕེལ་ཁ་ཆེ་བས་སེང་གེ་དང་འདྲ་བའོ། 19. དཔུང་པའི་མགོ་མགྲིན་པ་དང་འབྲེལ་ཞིང་ཟླུམ་པའོ། 20. ཐལ་གོང་རྒྱས་པ་ནི་བྲང་ངོ་ཞེས་ཤན་ཏི་སས་གསུངས་སོ། 21. རོ་བྲོ་བའི་མཆོག་མཁྱེན་པ་ནི། རྟ་ཆས་རུལ་བ་གསོལ་ཀྱང་རོ་མཆོག་ཏུ་སྣང་བའོ། 22. ཆུ་ཞེང་གབ་པ་ནི། སྐུའི་ཁྲུན་དང༌། འདོམ་གྱི་ཚད་དུ་མཉམ་པའོ། 23. སྐུ་སྨད་དང༌སྐུ་སྟོད་མཉམ་པ་སྟེ། ལྟེ་བ་ནས་བཟུང་སྟེ་སྐུ་སྟོད་སྐུ་སྨད་མཉམ་པའོ། 24. དབུ་གཙུག་ཏོར་དང་ལྡན་པ་ནི། ཕལ་པའི་ངོར་སོར་བཞི་འཕགས་པའོ། 25. ལྗགས་རིང་མཛེས་པ་ནི་ཞལ་གྱི་དཀྱིལ་འཁོར་ཁེབས་པའོ། 26. ཚངས་པའི་དབྱངས་ནི་ཉེ་རིང་ཐམས་ཅད་ལ་མཉམ་པར་གསལ་བའོ། 27. ཡང་ན་ཡན་ལག་ལྔ་དང་ལྡན་པ་སྟེ། ཤེས་ཤིང་རྣམ་པར་ཤེས་པར་འགྱུར་བ་དང་མཉམ་པར་འོས་ཤིང་མི་མཐུན་མེད་པ་དང་། ཟབ་ཅིང་རྗེས་སུ་སྒྲོག་པ་དང༌། མཚུངས་ཤིང་སྣང་བ་དང༌། རིག་ཅིང་རྣམ་པར་རིག་པར་བྱེད་པའོ། 28. འགྲམ་པ་སེང་གེ་འདྲ་བ་ནི་མེ་ལོང་ལྟར་མཐའ་བཟླུམ་ཞིང་རྒྱས་པའོ། 29. ཚེམས་ཐག་བཟང་བ་ནི་བར་མཚམས་མེད་པའོ། 30. བཞི་ཅུ་མངའ་བ་ནི། ཡས་མན་ཉི་ཤུ་རེ་མཉམ་པའོ། 31. སྤྱན་མཐོན་མཐིང་སྔོ་ནག་ཏུ་ཡོད་པའོ། 32. རྫི་མ་བའི་རྫི་མ་ལྟ་བུ་ནི་སྟེང་འོག་རྫི་མ་རྣམས་མ་འདྲེས་པའོ།</t>
+          <t>1. སྔོན་བླ་མ་རྣམས་ལ་བསྐྱལ་བ་དང་བསུ་བ་སོགས་བྱས་པས་ཕྱག་དང་ཞབས་འཁོར་ལོའི་རྩིབས་སྟོང་མུ་ཁྱུད་བཅས་པ་རྫོགས་པ་དང༌། 2. སྡོན་སྡོམ་པ་ཡང་དག་པར་བླངས་པ་བརྟན་པོར་བསྲུང་བས། ཞབས་རུས་སྦལ་བཞིན་དུ་མཉམ་པ། 3. སྔོན་བསྡུ་དངོས་བཞི་བརྟེན་པར་བྱས་པས་ཕྱག་དང་ཞབས་ཀྱི་སོར་མོ་ངང་པའི་རྒྱལ་པོ་ལྟ་བུར་རིན་པོ་ཆེའི་དྲ་བས་འབྲེལ་བ། 4. སྔོན་བཟའ་བ་དང་བཅའ་བ་བྱིན་པས། ཕྱག་དང་ཞབས་ཤིང་བལ་ལྟར་འཇམ་ཞིང་གཞོན་ཤ་ཆགས་པ། 5. བདུན་མཐོ་བ་ནི་ཕྱག་གི་བོལ་གཉིས། ཞབས་ཀྱི་བོལ་གཉིས་དཔུང་མགོ་གཉིས། ལྟག་པའི་ཕྱོགས་མཐོ་བའོ། 6. སོར་མོ་རིང་བ་ནི་ཞབས་མཐིལ་གྱི་དཀྱུས་དང་མཐོ་མཉམ་པའོ། 7. རྟིང་པ་ཡངས་པ་ནི་ཞབས་ཀྱི་བཞི་ཆ་ཕྱིར་འཕགས་པའོ། 8. སྟོན་པའི་སྐུའི་མཐོ་དམན་ནི། འཛམ་བུ་གླིང་པའི་ཁྲུ་ཕྱེད་དང་བཅུ་གཅིག་ཡོད་དོ། འཛམ་བུ་གླིང་པའི་མི་ལས་ཁྲུ་བདུན་ལྷག་པས་ན་སྐུ་ཆེ་ཞིང་དྲང་བའོ། 9. ཞབས་ཀྱི་ལོང་བུ་འབུར་བ་ཕྱིར་མི་མངོན་པའོ། 10. སྐུའི་སྤུ་གྱེན་དུ་འཁྱིལ་ཞིང་གཡས་སུ་ཕྱོགས་པ་དང་། 11. བྱིན་པ་རི་དྭགས་ཨེ་ན་ཡའི་ལྟ་བུ་ནི་ཡོངས་སུ་མཉམ་ཞིང་རིམ་པར་མཚམས་ལ་རྒྱས་ཤིང་བལྟམས་པའོ། 12.ཕྱག་རིང་བ་ནི། མ་བཅུད་པར་ཕྱག་གིས་པུས་མོའི་སླ་ངར་སླེབས་པའོ། 13. འདོམས་ཀྱི་སྦ་བ་སྦུབས་སུ་ནུབ་པ་ནི། གླང་པོ་ཆེའི་ལྟ་བུའོ། 14. གསེར་གྱི་མདངས་ལྟར་ཤིན་ཏུ་དྭངས་པའོ། 15. ལྤགས་པ་འཇམ་པ་ནི་གསེར་སྦྱངས་པ་ལྟར་སྙོམས་ལ་རྡུལ་གྱིས་མི་གོས་པའོ། 16. བ་སྤུའི་བུ་ག་གཅིག་ལ་གཉིས་མེད་པར་དོར་ན་གཡས་སུ་ལེགས་པར་འཁྲུངས་པ་དང་། 17. མཛོད་སྤུ་ནི་སྨིན་མཚམས་སུ་ས་དཀར་འཇམ་གཡས་སུ་འཁྱིལ་བ་ཉི་ཟླ་ལས་ལྷག་པའི་འོད་དང་ལྡན་པའོ། 18. སྐུའི་རོ་སྟོད་འཕེལ་ཁ་ཆེ་བས་སེང་གེ་དང་འདྲ་བའོ། 19. དཔུང་པའི་མགོ་མགྲིན་པ་དང་འབྲེལ་ཞིང་ཟླུམ་པའོ། 20. ཐལ་གོང་རྒྱས་པ་ནི་བྲང་ངོ་ཞེས་ཤན་ཏི་སས་གསུངས་སོ། 21. རོ་བྲོ་བའི་མཆོག་མཁྱེན་པ་ནི། རྟ་ཆས་རུལ་བ་གསོལ་ཀྱང་རོ་མཆོག་ཏུ་སྣང་བའོ། 22. ཆུ་ཞེང་གབ་པ་ནི། སྐུའི་ཁྲུན་དང༌། འདོམ་གྱི་ཚད</t>
         </is>
       </c>
       <c r="C2154" s="1" t="inlineStr">
@@ -36579,7 +36579,7 @@
       </c>
       <c r="B2168" s="1" t="inlineStr">
         <is>
-          <t>དགའ་བ་ཅན་གྱིས་ཞུས་པའི་མདོ་ལས། བཅོམ་ལྡན་འདས་ཀྱིས་གསུངས་པ། དགའ་བ་ཅན་འབྲུའི་ཆང་དང་བཅོས་པའི་ཆང་བག་མེད་པའི་གནས་ཀྱི་ཉེས་དམིགས་སུམ་ཅུ་སོ་ལྔ་ནི། འདི་དག་ཡིན་པས་རིག་པར་བྱ་སྟེ། སུམ་ཅུ་སོ་ལྔ་པོ་དེ་དག་གང་ཞེ་ན། 1. ཚེ་འདི་ལ་ནོར་ཟད་པ་དང༌། 2. ནད་རྣམས་རྒྱལ་བར་བྱེད་པ་དང༌། 3. འཐབ་པ་དང་རྩོད་པ་བསྐྱེད་པར་བྱེད་པ་དང༌། 4. དོན་མེད་པ་ལ་ལྟ་བ་དང༌། 5. གྲགས་པ་མ་ཡིན་ཀུན་འབྱུང་བར་བྱེད་པ་དང་། 6. ཤེས་རབ་ཉམ་ཆུང་བར་བྱེད་པ་དང་། 7. ལོངས་སྤྱོད་འཐོབ་པ་མི་འཐོབ་པར་འགྱུར་བ་དང༌། 8. ལོངས་སྤྱོད་ཐོབ་པ་ཡོངས་སུ་ཟད་ཅིང་ཡོངས་སུ་གཏུག་པར་འགྱུར་བ་དང་། 9. གསང་མི་ཐུབ་པར་འགྱུར་བ་དང༌། 10. དེའི་ལས་ཀྱི་མཐའ་ཡོངས་སུ་འགྲིབ་པ་དང་། 11. མཐུ་སྟོབས་ཆུང་ངུར་བྱེད་པར་འགྱུར་བ་དང༌། 12.མར་མི་འཛིན་པར་འགྱུར་བ་དང་། 13. ཕར་མི་འཛིན་པར་འགྱུར་བ་དང༌། 14. དགེ་སྦྱོང་དུ་མི་འཛིན་པར་འགྱུར་བ་དང༌། 15. བྲམ་ཟེར་མི་འཛིན་པར་འགྱུར་བ་དང༌། 16. རིགས་ཀྱི་གཙོ་བོ་ལ་བསྙེན་བསྐུར་མི་བྱེད་པར་འགྱུར་བ་དང་། 17. སངས་རྒྱས་ལ་མི་གུས་པར་འགྱུར་བ་དང་།18. ཆོས་ལ་མི་གུས་པར་འགྱུར་བ་དང༌། 19. དགེ་འདུན་ལ་མི་གུས་པར་འགྱུར་བ་དང་། 20. བསླབ་པ་ཡང་དག་པར་བླངས་པ་ལ་མ་གུས་པར་འགྱུར་བ་དང༌། 21. ཚུལ་ཁྲིམས་འཆལ་བར་འགྱུར་བ་དང་། 22. དབང་པོའི་སྒོ་མ་བསྡམས་པར་འགྱུར་བ་དང༌། 23. བག་མེད་པ་ལ་བུད་མེད་དོན་དུ་གཉེར་བར་འགྱུར་བ་དང་། 24. ཉེ་དུ་སྣག་གི་གཉེན་མཚམས་དང་མཛའ་བཤེས་དང་སློབ་དཔོན་དག་གིས་སྤོང་བར་འགྱུར་བ་དང༌། 25. སྐྱེ་བོ་མང་པོ་དག་གིས་ཡིད་དུ་མི་འོང་བར་འགྱུར་བ་དང༌། 26. སྐྱེ་བོ་མང་པོ་དག་དང་མི་མཐུན་པར་འགྱུར་བ་དང༌། 27. ཆོས་མ་ཡིན་པ་ལ་སྤྱོད་པར་འགྱུར་བ་དང༌། 28. ཆོས་མ་ཡིན་པ་ཡོངས་སུ་འཛིན་པར་འགྱུར་བ་དང༌། 29. དམ་པའི་ཆོས་ཡོངས་སུ་སྤོང་བར་འགྱུར་བ་དང་། 30. ངོ་ཚ་ཤེས་པ་དང་ཁྲེལ་ཡོད་པ་སྤོང་བར་འགྱུར་བ་དང་། 31. དེ་མི་མཛའ་བ་དག་དང་གནས་ཀྱང་མཁས་པ་རྣམས་ལ་ཡོངས་སུ་འདྲི་བར་མི་སེམས་པ་དང་།32. བག་མེད་ཉམས་བག་ཏུ་སྤྱོད་པར་འགྱུར་བ་དང༌།33. དེ་བཞིན་གཤེགས་པའི་གསུང་རབ་ལ་ཀུན་ནས་མི་གནས་པ་དང༌། 34. མྱ་ངན་ལས་འདས་པ་ལ་ཐག་རིང་དུ་འགྱུར་བ་དང་། 35. སྨྱོན་པར་འགྱུར་བའི་ལས་བྱས་ཤིང་བག་ཆགས་པས་ལུས་ཞིག་ནས་ངན་སོང་ངན་འགྲོ་ལོག་པར་ལྷུང་བ་སེམས་ཅན་དམྱལ་བ་དག་ཏུ་སྐྱེ་ཞིང་། གལ་ཏེ་དེ་ནས་ཤི་འཕོས་ཏེ་འདིར་མི་རྣམས་དང་སྐལ་བ་མཉམ་པར་སྐྱེས་ན་ཡང༌། དེ་དག་དང་གང་དུ་སྐྱེ་བ་དེ་དང་དེར་སྨྱོན་པར་འགྱུར་ཞིང་དྲན་པ་མི་གསལ་བར་གྱུར་ཏེ། དགའ་བ་འབྲུའི་ཆང་དང་བཅོས་པའི་ཆང་བག་མེད་པའི་གནས་ཀྱི་ཉེས་དམིགས་ནི་སུམ་ཅུ་རྩ་ལྔ་པོ་འདི་ཡིན་པར་རིག་པར་བྱའོ་ཞེས་གསུངས་སོ། ཡང་མདོ་དྲན་པ་ཉེར་བཞག་ལས། ཆང་གིས་གཡེང་བའི་མི་དག་ནི། གསོན་ཡང་ཤི་བ་དག་དང་མཚུངས་ཅེས་དང༌། དགེ་སྡིག་རྣམ་པར་འབྱེད་པའི་མདོ་ལས། ཚེ་འདི་ལ་ཆང་འཐུང་ཞིང་མྱོས་པ་ནི། ཟངས་ཁུ་འཐུང་བའི་དམྱལ་བར་ལྷུང་ངོ་། ཞེས་སོ།</t>
+          <t>དགའ་བ་ཅན་གྱིས་ཞུས་པའི་མདོ་ལས། བཅོམ་ལྡན་འདས་ཀྱིས་གསུངས་པ། དགའ་བ་ཅན་འབྲུའི་ཆང་དང་བཅོས་པའི་ཆང་བག་མེད་པའི་གནས་ཀྱི་ཉེས་དམིགས་སུམ་ཅུ་སོ་ལྔ་ནི། འདི་དག་ཡིན་པས་རིག་པར་བྱ་སྟེ། སུམ་ཅུ་སོ་ལྔ་པོ་དེ་དག་གང་ཞེ་ན། 1. ཚེ་འདི་ལ་ནོར་ཟད་པ་དང༌། 2. ནད་རྣམས་རྒྱལ་བར་བྱེད་པ་དང༌། 3. འཐབ་པ་དང་རྩོད་པ་བསྐྱེད་པར་བྱེད་པ་དང༌། 4. དོན་མེད་པ་ལ་ལྟ་བ་དང༌། 5. གྲགས་པ་མ་ཡིན་ཀུན་འབྱུང་བར་བྱེད་པ་དང་། 6. ཤེས་རབ་ཉམ་ཆུང་བར་བྱེད་པ་དང་། 7. ལོངས་སྤྱོད་འཐོབ་པ་མི་འཐོབ་པར་འགྱུར་བ་དང༌། 8. ལོངས་སྤྱོད་ཐོབ་པ་ཡོངས་སུ་ཟད་ཅིང་ཡོངས་སུ་གཏུག་པར་འགྱུར་བ་དང་། 9. གསང་མི་ཐུབ་པར་འགྱུར་བ་དང༌། 10. དེའི་ལས་ཀྱི་མཐའ་ཡོངས་སུ་འགྲིབ་པ་དང་། 11. མཐུ་སྟོབས་ཆུང་ངུར་བྱེད་པར་འགྱུར་བ་དང༌། 12.མར་མི་འཛིན་པར་འགྱུར་བ་དང་། 13. ཕར་མི་འཛིན་པར་འགྱུར་བ་དང༌། 14. དགེ་སྦྱོང་དུ་མི་འཛིན་པར་འགྱུར་བ་དང༌། 15. བྲམ་ཟེར་མི་འཛིན་པར་འགྱུར་བ་དང༌། 16. རིགས་ཀྱི་གཙོ་བོ་ལ་བསྙེན་བསྐུར་མི་བྱེད་པར་འགྱུར་བ་དང་། 17. སངས་རྒྱས་ལ་མི་གུས་པར་འགྱུར་བ་དང་།18. ཆོས་ལ་མི་གུས་པར་འགྱུར་བ་དང༌། 19. དགེ་འདུན་ལ་མི་གུས་པར་འགྱུར་བ་དང་། 20. བསླབ་པ་ཡང་དག་པར་བླངས་པ་ལ་མ་གུས་པར་འགྱུར་བ་དང༌། 21. ཚུལ་ཁྲིམས་འཆལ་བར་འགྱུར་བ་དང་། 22. དབང་པོའི་སྒོ་མ་བསྡམས་པར་འགྱུར་བ་དང༌། 23. བག་མེད་པ་ལ་བུད་མེད་དོན་དུ་གཉེར་བར་འགྱུར་བ་དང་། 24. ཉེ་དུ་སྣག་གི་གཉེན་མཚམས་དང་མཛའ་བཤེས་དང་སློབ་དཔོན་དག་གིས་སྤོང་བར་འགྱུར་བ་དང༌། 25. སྐྱེ་བོ་མང་པོ་དག་གིས་ཡིད་དུ་མི་འོང་བར་འགྱུར་བ་དང༌། 26. སྐྱེ་བོ་མང་པོ་དག་དང་མི་མཐུན་པར་འགྱུར་བ་དང༌། 27. ཆོས་མ་ཡིན་པ་ལ་སྤྱོད་པར་འགྱུར་བ་དང༌། 28. ཆོས་མ་ཡིན་པ་ཡོངས་སུ་འཛིན་པར་འགྱུར་བ་དང༌། 29. དམ་པའི་ཆོས་ཡོངས་སུ་སྤོང་བར་འགྱུར་བ་དང་། 30. ངོ་ཚ་ཤེས་པ་དང་ཁྲེལ་ཡོད་པ་སྤོང་བར་འགྱུར་བ་དང་། 31. དེ་མི་མཛའ་བ་དག་དང་གནས་ཀྱང་མཁས་པ་རྣམས་ལ་ཡོངས་སུ་འདྲི་བར་མི་སེམས་པ་དང་།32. བག་མེད་ཉམས་བག་ཏུ་སྤྱོད་པར་འགྱུར་བ་དང༌།33. དེ་བཞིན་གཤེགས་པའི་གསུང་རབ་ལ་ཀུན་ནས་མི་གནས་པ་དང༌། 34. མྱ་ངན་ལས་འདས་པ་ལ་ཐག་རིང་དུ་འགྱུར་བ་དང་། 35. སྨྱོན་པར་འགྱུར་བའི་ལས་བྱས་ཤིང་བག་ཆགས་པས་ལུས་ཞིག་ནས་ངན་སོང་ངན་འགྲོ་ལོག་པར་ལྷུང་བ་སེམས་ཅན་དམྱལ་བ་དག་ཏུ་སྐྱེ་ཞིང་། གལ་ཏེ་དེ་ནས་ཤི་འཕོས་ཏེ་འདིར་མི་རྣམས་དང་སྐལ་བ་མཉམ་པར་སྐྱེས་ན་ཡང༌། དེ་དག་དང་གང་དུ་སྐྱེ་བ་དེ་དང་དེར་སྨྱོན་པར་འགྱུར་ཞིང་དྲན་པ་མི་གསལ་བར་གྱུར་ཏེ། དགའ་བ་འབྲུའི་ཆང་དང་བཅོས་པའི་ཆང་བག་མེད་པའི་གནས་ཀྱི་ཉེས་དམིགས་ནི་སུམ་ཅུ་རྩ་ལྔ་པོ་འདི་ཡིན་པར་རིག་པར་བྱའོ་ཞེས་གསུངས་སོ། ཡང་མདོ་དྲན་པ་ཉེར་བཞག་ལས། ཆང་གིས་གཡེང་བའི་མི་དག་ནི། གསོན་ཡང་ཤི་བ་དག་དང་མཚུངས་ཅེས་དང༌། དགེ་སྡིག་རྣམ་པར་འབྱེད་པའི་མདོ་ལས། ཚེ་འདི་ལ་ཆང་འཐུང་ཞིང</t>
         </is>
       </c>
       <c r="C2168" s="1" t="inlineStr">
@@ -36970,7 +36970,7 @@
       </c>
       <c r="B2191" s="1" t="inlineStr">
         <is>
-          <t>སངས་རྒྱས་ཆོས་ལུགས་ཀྱི་བཤད་སྲོལ་ལ། གསང་སྔགས་ཀྱི་ལམ་ལ་བརྟེན་ནས་ཐུན་མོང་གི་དངོས་གྲུབ་བརྒྱད་དམ། སྐུ་ཚེ་དེ་ལ་སངས་རྒྱས་པའམ། མཆོག་གི་དངོས་གྲུབ་གང་རུང་ཐོབ་པ་ལ་གྲུབ་ཐོབ་དང་གྲུབ་ཆེན་ཟེར། གྲུབ་ཆེན་འདི་རྣམས་དུས་སྐབས་གང་དུ་བྱུང་བ་ན། ཇོ་ནང་ཏཱ་ར་ན་ཐས་བརྩམས་པའི་《རྒྱ་གར་ཆོས་འབྱུང་》ལས། ནང་པའི་སློབ་དཔོན་གྲུབ་ཐོབ་བརྒྱད་ཅུ་རྩ་བཞིར་གྲགས་པ་ཕྱེད་ལྷག་ཙམ་སློབ་དཔོན་ཆོས་གྲགས་ཀྱི་དུས་མན་ཆད་ནས་རྒྱལ་པོ་ཙ་ན་ཀས་སྲིད་དབང་བཟུང་བ་ཡན་ཆད་དུ་བྱོན་པ་དང༌། རྒྱལ་པོ་གོ་པཱ་ལ་ནས་རཱ་མ་པཱ་ལའི་བར་པཱ་ལ་བདུན་བརྒྱུད་ཀྱི་རིང་གསང་སྔགས་ཀྱི་ལམ་ལ་བརྟེན་ནས་གྲུབ་པ་ཐོབ་པ་ཤིན་ཏུ་མང་བར་བྱོན་ཞེས་བཤད་པ་ལྟར་ན། གྲུབ་ཐོབ་བརྒྱད་ཅུ་རྩ་བཞིའི་ནང་གི་མང་ཆེ་བ་བོད་ཀྱི་རབ་བྱུང་གོང་གི་ཤཱཀྱུའི་འདས་ལོ་(འདིའི་ནང་གི་ཤཱཀྱའི་འདས་ལོ་རྣམས་ཁ་ཆེ་པཎ་ཆེན་ཤཱཀྱ་བྐྲིའི་ལུགས་ཀྱི་འདས་ལོ་གཞིར་བཟུང་བ་ཡིན）1165 ལོ——བོད་ཀྱི་རབ་བྱུང་གསུམ་པའི་མཇུག་བར་དང་། སྤྱི་ལོའི་དུས་རབས་བདུན་པ་ནས་དུས་རབས་བཅུ་གཉིས་པའི་མཇུག་བར་གྱི་ལོ་དྲུག་བརྒྱ་ཐམ་པའི་རིང་དེར་བྱུང་བར་མངོན། འདིར་གྲུབ་ཐོབ་བརྒྱད་ཅུ་རྩ་བཞིའི་མིང་ཙམ་སྨོས་ན། 1. ལུ་ཨི་པ། ཉ་ལྟོ་བ། 2. དྷ་རི་ཀ་པ། སྨད་འཚོང་ལ་གཡོག་བྱེད་པ། 3. ཌིམ་ཀེ་པ། 4. ལི་ལ་པ། 5. བིར་ཝ་བ། དཔལ་ལྡན་ཆོས་སྐྱོང་། 6.ཊོམ་བྷི་བ། 7. ཤ་ཝ་རི་པ། རི་དྭགས་རྔོན་པ། 8. ས་ར་ཧ་པ། བྲམ་བྲེས་ར་ཧ་པ། 9. ཀོ་ཀ་ལི་བ། ཉལ་པོ་ལ་དགའ་བ། 10. མི་ན་པ། ཉ་པ། 11. གོ་རཀྵ་པ། རྐང་ལག་མེད་པ། 12. ཙ་འུར་ཁ་པ། བ་ལང་སྐྱོང་། 13. བི་ན་པ། རོ་མོ་ལ་ཆགས་པ། 14. རཧྣ་ཨ་ཀ་ར་ཤནྷི། རིན་ཆེན་འབྱུང་གནས་ཞི་བ། 15. ཏོག་ཙེ་པ། འཇོར་ཐོགས་མཁན། 16. ཧཎྚི་པ། ཐགས་མཁན། 17. ཙ་མ་རི་པ། ལྷམ་མཁན། 18. ཁངྒ་པ། རལ་གྲི་ཅན། 19. ཀླུ་སྒྲུབ་སློབ་དཔོན། ཀླུ་སྒྲུབ། 20. ཀཧྞི་པ། ནག་པོ་སྤྱོད་པ། 21. ཀ་ན་རི་པ། སློབ་དཔོན་ཨརྱ་དེ་བ། 22. ཐེ་གེ་ན་པ། བརྫུན་ལ་དགའ་བ། 23. ཏེ་ལོ་པ། ཏིལ་བརྡུང་མཁན། 24. ནཱ་རོ་པ། པཎ་ཆེན་ནཱ་རོ་པ། 25. ཤ་ལི་པ། སྤྱང་ཀི་པ། 26. ཙ་ཏ་པ། ཆོས་སློང་མཁན། 27. བྷ་ཧ་པ། 28. དྷོ་ཁན་དྷི་པ། 29.ཨ་ཛུ་ཀི ལེ་ལོ་ཅན། 30. ས་ཀ་ལ་པ། སྨྱོན་པ། 31. ཌོམ་བི་བ། ཁྲུས་མཁན། 32. མེ་ཀོ་པ། དུར་ཁྲོད་པ། 33. ཀ་མ་རི་པ། མགར་བ། 34. ཛ་ལན་དྷ་ར་པ། འབར་བ་འཛིན། 35. ར་ཧུ་ལ། སྒྲ་གཅན་འཛིན། 36. དྷ་རྨ་པ། ཆོས་སྨྲ་བ། ། 37. དྷོ་ཀ་རི་པ། སྣོད་འཁུར་བ། 38. མེ་དྷ་ནི། ཞིང་པ། 39. སདྷ་ཛ་ལ། 40. དྲིལ་བུ་པ། 41. ཨ་ཡོ་གི 42. ཙ་ལོ་གི 43. གུ་ཧུ་རི་པ། བྱ་པ། 44. ལུ་ཙི་ཀ ཙོག་འདུག་ལྐོག་ལངས། 45. ཀམ་ཀ་ལ། གདུ་བུ་པ། 46. ཀམ་པ་ལི། ལ་ཝ་པ། 47. བྷ་དེ་པ། 48. ཏེན་ཏ་པ། ཆོ་ལོ་པ། 49. ཀུ་ཀུ་རི་པ། ཁྱི་ལ་དགའ་བ། 50. ཀུ་ཛྙ་ལི། ལྟག་ཝ་ཅན། 51. དྷརྨ་པ། ཐོས་ཤེས་ཅན། 52. མ་དྷི་ལ། ང་རྒྱལ་ཅན། 53. ཨ་ཙི་ཎྟ། ཤིང་འཚོང་མཁན། 54. བྷ་ལ་ཧ། 55. ན་ལི་པ། འདམ་གྱིས་གམ་གོས་པའི་པདྨ། 56. བྷུ་སུ་ཀུ་པ། འདུ་ཤེས་གསུམ་པ། 57. ཨིནྡྲ་བོ་དྷི། བྱང་ཆུབ་དབང་པོ། 58. ལེགས་སྨིན་ཀ་ར། དེའི་སྐུ་མཆེད་(མོ） 59. ཛ་ལེནྡྲ་པ། འབར་བའི་དབང་པོ། 60. ནི་ར་གུ་ན། ཡོན་ཏན་མེད་པ། 61. ཙ་བ་རི་པ། འཁུར་པ་འཚོང་བ། 62. ཙ་པ་ཀ 63. བྷི་ཁ་ན། 64. ཏིལ་བརྡུང་པ། 65. ཀུ་མ་རི། 66. དུ་མེ་བ། 67. མ་ཎི་བྷ་དྲ་ (མོ） 68. རྣལ་འབྱོར་མ་མེ་ཁ་ལ། 69. དེའི་སྐུ་མཆེད་(མོ) 70. ཀ་ན་ཀ་པ། མུ་ཅོར་སྨྲ་བ། 71. ཀུན་ཐ་ལི་པ། འཚེམ་བུ་པ། 72. དྷ་པུ་རི་པ། ཀུ་ཤའི་ཐག་པ་གཅུ་མཁན། 73. ཨུ་དྷ་རི་པ། རྫུ་འཕྲུལ་གྱིས་འཕུར་མཁན། 74. ཀ་པཱ་ལི་པ། ཐོད་པ་ཅན། 75. ཀི་ར་པ། སྲིད་དམག་ལ་དགའ་བ། 76. མཚོ་སྐྱེས་རྡོ་རྗེ། 77. སྭརྦ་བྷ་ག་ལ། མཐོང་ཚད་ཟ་བ། 78. ན་ག་བོ་དྷི། ཀླུ་བྱང་ཆུབ། 79. ཁུང་ལི་པ། བྲིས་སྐུ་འཆང་བ། 80. པ་ན་ཧ། མཆིལ་ལྷམ་ཅན། 81. ཀོ་ཀ་ལི་པ། བྱ་ཀོ་ཀ་ལི་ལ་དགའ་བ། 82. ཨ་ན་ཀ ལུས་བཟང་པ། 83. སམུནྡྲ། ཚོང་བྱེད་མཁན། 84. བྱ་རི་པ། བཅུད་ལེན་མཁན་བཅས་ཡིན། སྤྱིར་གསང་སྔགས་བླ་མེད་ཀྱི་ལམ་ལ་བརྟེན་ནས་གྲུབ་པ་ཐོབ་པ་ནི་སློབ་དཔོན་ཀླུ་སྒྲུབ་ཀྱི་དུས་ཁོ་ནར་ལྔ་སྟོང་ལྷག་ཙམ་བྱུང་བར་བཤད་ཅིང་། ཡོངས་གྲགས་སུ་གྲུབ་ཐོབ་བརྒྱད་ཅུ་རྩ་བཞི་དང་གྲུབ་ཐོབ་བརྒྱད་ཅུ་ཞེས་གྲགས་པ་ནི། བླ་མ་རྡོ་རྗེ་གདན་པས་ཚོགས་འཁོར་མཛད་པའི་སྐབས་དངོས་སུ་བྱོན་པའི་གྲུབ་ཐོབ་ཀྱི་གྲངས་ལ་བརྒྱད་ཅུ་བྱུང་བར་བརྟེན་ནས་མིང་དེ་ལྟར་གྲགས་པ་ཡིན་ཟེར་སྲོལ་ཡོད།</t>
+          <t>སངས་རྒྱས་ཆོས་ལུགས་ཀྱི་བཤད་སྲོལ་ལ། གསང་སྔགས་ཀྱི་ལམ་ལ་བརྟེན་ནས་ཐུན་མོང་གི་དངོས་གྲུབ་བརྒྱད་དམ། སྐུ་ཚེ་དེ་ལ་སངས་རྒྱས་པའམ། མཆོག་གི་དངོས་གྲུབ་གང་རུང་ཐོབ་པ་ལ་གྲུབ་ཐོབ་དང་གྲུབ་ཆེན་ཟེར། གྲུབ་ཆེན་འདི་རྣམས་དུས་སྐབས་གང་དུ་བྱུང་བ་ན། ཇོ་ནང་ཏཱ་ར་ན་ཐས་བརྩམས་པའི་《རྒྱ་གར་ཆོས་འབྱུང་》ལས། ནང་པའི་སློབ་དཔོན་གྲུབ་ཐོབ་བརྒྱད་ཅུ་རྩ་བཞིར་གྲགས་པ་ཕྱེད་ལྷག་ཙམ་སློབ་དཔོན་ཆོས་གྲགས་ཀྱི་དུས་མན་ཆད་ནས་རྒྱལ་པོ་ཙ་ན་ཀས་སྲིད་དབང་བཟུང་བ་ཡན་ཆད་དུ་བྱོན་པ་དང༌། རྒྱལ་པོ་གོ་པཱ་ལ་ནས་རཱ་མ་པཱ་ལའི་བར་པཱ་ལ་བདུན་བརྒྱུད་ཀྱི་རིང་གསང་སྔགས་ཀྱི་ལམ་ལ་བརྟེན་ནས་གྲུབ་པ་ཐོབ་པ་ཤིན་ཏུ་མང་བར་བྱོན་ཞེས་བཤད་པ་ལྟར་ན། གྲུབ་ཐོབ་བརྒྱད་ཅུ་རྩ་བཞིའི་ནང་གི་མང་ཆེ་བ་བོད་ཀྱི་རབ་བྱུང་གོང་གི་ཤཱཀྱུའི་འདས་ལོ་(འདིའི་ནང་གི་ཤཱཀྱའི་འདས་ལོ་རྣམས་ཁ་ཆེ་པཎ་ཆེན་ཤཱཀྱ་བྐྲིའི་ལུགས་ཀྱི་འདས་ལོ་གཞིར་བཟུང་བ་ཡིན）1165 ལོ——བོད་ཀྱི་རབ་བྱུང་གསུམ་པའི་མཇུག་བར་དང་། སྤྱི་ལོའི་དུས་རབས་བདུན་པ་ནས་དུས་རབས་བཅུ་གཉིས་པའི་མཇུག་བར་གྱི་ལོ་དྲུག་བརྒྱ་ཐམ་པའི་རིང་དེར་བ</t>
         </is>
       </c>
       <c r="C2191" s="1" t="inlineStr">
@@ -36987,7 +36987,7 @@
       </c>
       <c r="B2192" s="1" t="inlineStr">
         <is>
-          <t>ལྟུང་བྱེད་འབའ་ཞིག་ཏུ་འགྱུར་བ་རྣམས་ལ། བཅུ་བ་དང་པོ་ལ། 1. བརྫུན། 2. སྐྱོན་ནས་སྨྲ་བ། 3. དགེ་སློང་ལ་ཕྲ་མ་བྱེད་པ། 4. སྐྱོ་སྔོགས་བྱེད་པ། 5. གནས་ངན་ལེན་བྱེད་པ། 6. མིའི་ཆོས་བླ་མ་བརྗོད་པ། 7. ཚིག་དྲུག་གམ་ལྔ་ནས་ལྷག་པར་ཆོས་བཤད་ན། 8. ཚིག་མཐུན་དང༌ཚིག་ལྷག་པར་སློབ་པ། 9. ཤེས་ངོར་བྱེད་པ། 10. ཁྱད་དུ་གསོད་པ། བཅུ་བ་གཉིས་པ་ལ། 11. ས་བོན་གྱི་ཚོགས་དང་འབྱུང་པོའི་ཚོགས་འཇིགས་པ། 12. འཕྱ་བ། 13. བསྒོ་བ་བཅག་པ། 14. ཁྲི། 15. གདིང་བ། 16. སྐྲོད་པ། 17. ཕྱིས་མནན་པ། 18. རྩ་བ་འབྱུང་བ་ལ་འདུག་པ། 19. སྲོག་ཆགས་དང་བཅས་པ་ལ་སྤྱོད་པ། 20. རིམ་གཉིས་སམ་གསུམ་བརྩིག་པ། བཅུ་པ་གསུམ་པ་ལ། 21. མ་བསྐོས་པར་སྟོན་པ། 22. ཉི་མ་ནུབ་ཀྱི་བར་དུ་སྟོན་པ། 23. ཟས་ཅུང་ཟད་ཙམ་གྱི་ཕྱིར་སྟོན་པ། 24. གོས་སྦྱིན་པ། 25. གོས་འཚེམ་པ། 26. དགེ་སློང་མའི་མགྲོན་པ་མང་པོ་དང་ལྷན་ཅིག་འགྲོ་བ། 27. དགེ་སློང་མ་དང་ལྷན་ཅིག་གྲུར་འཇུག་པ། 28. དབེན་པ་ན་འདུག་པ། 29. དབེན་པ་ན་འགྲེང་བ། 30. དགེ་སློང་མས་སྦྱོར་དུ་བཅུག་པའི་ཟས་ཟ་བ། བཅུ་བ་བཞི་པ་ལ། 31. ཡང་ཡང་ཟ་བ། 32. གནས་གཅིག་ན་གནས་པ། 33. ལྷུང་བཟེད་དོ་གསུམ་ལས་ལྷག་པར་ལེན་པ། 34. ལྷག་མར་མ་བྱས་པའི་བཟའ་བ། 35. ལྷག་པར་མ་བྱས་པའི་སྟོབས། 36. འདུས་ཤིང་ཟ་བ། 37. དུས་མ་ཡིན་པར་ཟ་བ། 38. གསོག་འཇོག་སྤང་བ། 39. སྦྱིན་ལེན་མ་བྱས་པར་ཟ་བ། 40. ཟས་གསོད་པ་སྤོང་བ། བཅུ་བ་ལྔ་པ་ལ། 41. སྲོག་ཆགས་དང་བཅས་པའི་ཆུ་ལ་སྤྱོད་པ། 42. ཉལ་པོ་བྱེད་པོ་གཤོམ་པའི་ཁྱིམ་ན་གནས་པ། 43. ཉལ་པོ་བྱེད་པར་གཤོམ་པའི་ཁྱིམ་ན་འགྲེང་བ། 44. གཅེར་བུ་བ་ལ་སྦྱིན་པ། 45. དམག་ལ་བལྟ་བ། 46. དམག་གི་ནང་ན་གནས་པ། 47. གཡུལ་བཤམས་པ་འཁྲུགས་སུ་འགྲོ་བ། 48. བརྡེག་པ། 49.གཟས་པ། 50. གནས་ངན་ལེན་འཆབ་པ། བཅུ་བ་དྲུག་པ་ལ། 51. ཟས་གཅོད་དུ་འཇུག་པ། 52. མེ་འཁུད་པ། 53. དད་པ་ཕྱིར། 54. བསྙེན་པར་མ་རྫོགས་པ་དང་ལྷན་ཅིག་ཉལ་བ། 55. ལྟ་བར་འགྱུར་བ་མི་འདོར་བ། 56. སྤངས་པའི་རྗེས་སུ་ཕྱོགས་པ། 57. བསྙིལ་བ་སྡུད་པ། 58. ཁ་མ་བསྒྱུར་པའི་གོས་གྱོན་པ། 59. རིན་པོ་ཆེ་ལ་རག་པ། 60. ཁྲུས་བྱེད་པ་ལྟུང་བྱེད། བཅུ་བ་བདུན་པ་ལ། 61. དུད་འགྲོ་གསོད་པ། 62. འགྱོད་པ་བསྐྱེད་པ། 63. མཛུབ་མོས་ག་ག་ཚིལ་བྱེད་པ། 64. ཆུ་ལ་རྩེ་བ། 65. བུད་མེད་དང་ལྷན་ཅིག་ཉལ་བ། 66. སྔངས་པར་བྱེད་པ། 67. སྤེད་པ། 68. ཕྱིར་མ་བླང་པར་སྤྱོད་པ། 69. གཞི་མེད་པ་སྐུར་བར་འདེབས་པ། 70. སྐྱེས་པ་མེད་པའི་བུད་མེད་དང་ལམ་དུ་འགྲོ་བ། བཅུ་བ་བརྒྱད་པ་ལ། 71. རྐུན་མ་དང་ལྷན་ཅིག་འགྲོ་བ། 72. ཉི་ཤུ་མ་ལོན་པར་བསྙེན་པར་རྫོགས་པར་བྱེད་པ། 73. ས་བརྐོ་བ། 74. མགྲོན་གཉེར་བ་ལས་རིང་དུ་འདུག་པ། 75. ཉན་རྣ་ལས་གྱུར་པ། 76. བསླབ་པ་ཉེ་བར་འཇོག་པ་སྤང་བ། 77. མི་སྨྲ་བར་འགྲོ་བ། 78. མ་གུས་པའི་ཚུལ། 79. འབྲུའི་ཆང་དང་སྦྱར་བའི་ཆང་མྱོས་པར་གྱུར་བ་འཐུང་བ། 80. དུས་མ་ཡིན་པར་འགྲོ་བ། བཅུ་བ་དགུ་བ་ལ། 81. གྲོང་རྒྱུ་བ། 82. རྒྱལ་པོའི་ཕོ་བྲང་དུ་ནུབ་མོ་འགྲོ་བ། 83. བསླབ་པའི་ཚིག་གི་དངོས་པོ་ཁྱད་དུ་གསོད་པ། 84. ཁབ་རལ་འཚོས་པ། 85. ཁྱིའི་རྐང་པ་འཚོས་པ། 86. ཤིང་བལ་གྱིས་གོས་པར་བྱ་བ། 87. གདིངས་པ་ལས་གྱུར་པ། 88. དབྱར་གྱི་རས་ཆེན་ལས་གྱུར་པ། 89. གཡན་པ་དགབ་པ་ལས་གྱུར་བ། 90. བདེ་བར་གཤེགས་པའི་གོས་ཀྱི་ཚད་ལས་གྱུར་བ།</t>
+          <t>ལྟུང་བྱེད་འབའ་ཞིག་ཏུ་འགྱུར་བ་རྣམས་ལ། བཅུ་བ་དང་པོ་ལ། 1. བརྫུན། 2. སྐྱོན་ནས་སྨྲ་བ། 3. དགེ་སློང་ལ་ཕྲ་མ་བྱེད་པ། 4. སྐྱོ་སྔོགས་བྱེད་པ། 5. གནས་ངན་ལེན་བྱེད་པ། 6. མིའི་ཆོས་བླ་མ་བརྗོད་པ། 7. ཚིག་དྲུག་གམ་ལྔ་ནས་ལྷག་པར་ཆོས་བཤད་ན། 8. ཚིག་མཐུན་དང༌ཚིག་ལྷག་པར་སློབ་པ། 9. ཤེས་ངོར་བྱེད་པ། 10. ཁྱད་དུ་གསོད་པ། བཅུ་བ་གཉིས་པ་ལ། 11. ས་བོན་གྱི་ཚོགས་དང་འབྱུང་པོའི་ཚོགས་འཇིགས་པ། 12. འཕྱ་བ། 13. བསྒོ་བ་བཅག་པ། 14. ཁྲི། 15. གདིང་བ། 16. སྐྲོད་པ། 17. ཕྱིས་མནན་པ། 18. རྩ་བ་འབྱུང་བ་ལ་འདུག་པ། 19. སྲོག་ཆགས་དང་བཅས་པ་ལ་སྤྱོད་པ། 20. རིམ་གཉིས་སམ་གསུམ་བརྩིག་པ། བཅུ་པ་གསུམ་པ་ལ། 21. མ་བསྐོས་པར་སྟོན་པ། 22. ཉི་མ་ནུབ་ཀྱི་བར་དུ་སྟོན་པ། 23. ཟས་ཅུང་ཟད་ཙམ་གྱི་ཕྱིར་སྟོན་པ། 24. གོས་སྦྱིན་པ། 25. གོས་འཚེམ་པ། 26. དགེ་སློང་མའི་མགྲོན་པ་མང་པོ་དང་ལྷན་ཅིག་འགྲོ་བ། 27. དགེ་སློང་མ་དང་ལྷན་ཅིག་གྲུར་འཇུག་པ། 28. དབེན་པ་ན་འདུག་པ། 29. དབེན་པ་ན་འགྲེང་བ། 30. དགེ་སློང་མས་སྦྱོར་དུ་བཅུག་པའི་ཟས་ཟ་བ། བཅུ་བ་བཞི་པ་ལ། 31. ཡང་ཡང་ཟ་བ། 32. གནས་གཅིག་ན་གནས་པ། 33. ལྷུང་བཟེད་དོ་གསུམ་ལས་ལྷག་པར་ལེན་པ། 34. ལྷག་མར་མ་བྱས་པའི་བཟའ་བ། 35. ལྷག་པར་མ་བྱས་པའི་སྟོབས། 36. འདུས་ཤིང་ཟ་བ། 37. དུས་མ་ཡིན་པར་ཟ་བ། 38. གསོག་འཇོག་སྤང་བ། 39. སྦྱིན་ལེན་མ་བྱས་པར་ཟ་བ། 40. ཟས་གསོད་པ་སྤོང་བ། བཅུ་བ་ལྔ་པ་ལ། 41. སྲོག་ཆགས་དང་བཅས་པའི་ཆུ་ལ་སྤྱོད་པ། 42. ཉལ་པོ་བྱེད་པོ་གཤོམ་པའི་ཁྱིམ་ན་གནས་པ། 43. ཉལ་པོ་བྱེད་པར་གཤོམ་པའི་ཁྱིམ་ན་འགྲེང་བ། 44. གཅེར་བུ་བ་ལ་སྦྱིན་པ། 45. དམག་ལ་བལྟ་བ། 46. དམག་གི་ནང་ན་གནས་པ། 47. གཡུལ་བཤམས་པ་འཁྲུགས་སུ་འགྲོ་བ། 48. བརྡེག་པ། 49.གཟས་པ། 50. གནས་ངན་ལེན་འཆབ་པ། བཅུ་བ་དྲུག་པ་ལ། 51. ཟས་གཅོད་དུ་འཇུག་པ། 52. མེ་འཁུད་པ། 53. དད་པ་ཕྱིར། 54. བསྙེན་པར་མ་རྫོགས་པ་དང་ལྷན་ཅིག་ཉལ་བ། 55. ལྟ་བར་འགྱུར་བ</t>
         </is>
       </c>
       <c r="C2192" s="1" t="inlineStr">

</xml_diff>